<commit_message>
Point Sheet components structured / able to create/read documents from database / delete/update documents functionality not implemented yet / python scripts added for writing to database, generating spreadsheet, and emailing spreadsheets / node used to retrieve documents / no styling yet
</commit_message>
<xml_diff>
--- a/client/test.xlsx
+++ b/client/test.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="164">
   <si>
     <t>Greenville Convention Center - Alcohol Point Sheets</t>
   </si>
@@ -36,54 +36,33 @@
     <t>Event Number and Name:</t>
   </si>
   <si>
-    <t>Ballers Bar</t>
-  </si>
-  <si>
     <t>Date of Function</t>
   </si>
   <si>
-    <t>10/24/2018</t>
-  </si>
-  <si>
     <t>Bartender(s):</t>
   </si>
   <si>
-    <t>Taylor Mosier, Candice Overcash</t>
-  </si>
-  <si>
     <t>Room:</t>
   </si>
   <si>
-    <t>Exhibit Hall B</t>
-  </si>
-  <si>
     <t>Host Bar (Y/N)</t>
   </si>
   <si>
-    <t>y</t>
-  </si>
-  <si>
     <t>Sales Tax Percentage</t>
   </si>
   <si>
-    <t>7%</t>
-  </si>
-  <si>
     <t>7.00% is default</t>
   </si>
   <si>
     <t>Service Charge Percentage</t>
   </si>
   <si>
-    <t>21%</t>
+    <t>20.00% is default</t>
   </si>
   <si>
     <t>If Cash Bar - Actual Cash Collected:</t>
   </si>
   <si>
-    <t>$1400.00</t>
-  </si>
-  <si>
     <t>PRICES (INCLUDING TAX)</t>
   </si>
   <si>
@@ -102,36 +81,24 @@
     <t>Call</t>
   </si>
   <si>
-    <t>$6</t>
-  </si>
-  <si>
     <t>Premium Liquor (Prem)</t>
   </si>
   <si>
     <t>Prem</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
     <t>Top Shelf Premium Liquor (Top)</t>
   </si>
   <si>
     <t>Top</t>
   </si>
   <si>
-    <t>$9</t>
-  </si>
-  <si>
     <t>Well Liquor (Top)</t>
   </si>
   <si>
     <t>Well</t>
   </si>
   <si>
-    <t>$5</t>
-  </si>
-  <si>
     <t>Number of oz per shot (Calculated/Default)</t>
   </si>
   <si>
@@ -162,9 +129,6 @@
     <t>Dom</t>
   </si>
   <si>
-    <t>$4</t>
-  </si>
-  <si>
     <t>Imported Beer</t>
   </si>
   <si>
@@ -174,9 +138,6 @@
     <t>Greenville Convention Center      Bar Point Sheet</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Revenue Calculation</t>
   </si>
   <si>
@@ -234,6 +195,9 @@
     <t>Aristocrat Vodka</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>Smirnoff</t>
   </si>
   <si>
@@ -262,9 +226,6 @@
   </si>
   <si>
     <t>Gordons</t>
-  </si>
-  <si>
-    <t>11</t>
   </si>
   <si>
     <t>Tanqueray</t>
@@ -1625,103 +1586,91 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="n"/>
-      <c r="C5" s="112" t="s">
-        <v>4</v>
-      </c>
+      <c r="C5" s="112" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="6" spans="1:5">
       <c r="A6" s="21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="21" t="n"/>
-      <c r="C6" s="144" t="s">
-        <v>6</v>
-      </c>
+      <c r="C6" s="144" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="7" spans="1:5">
       <c r="A7" s="21" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" s="21" t="n"/>
-      <c r="C7" s="112" t="s">
-        <v>8</v>
-      </c>
+      <c r="C7" s="112" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="8" spans="1:5">
       <c r="A8" s="21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8" s="21" t="n"/>
-      <c r="C8" s="112" t="s">
-        <v>10</v>
-      </c>
+      <c r="C8" s="112" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="9" spans="1:5">
       <c r="A9" s="21" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" s="21" t="n"/>
-      <c r="C9" s="112" t="s">
-        <v>12</v>
-      </c>
+      <c r="C9" s="112" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="10" spans="1:5">
       <c r="A10" s="21" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B10" s="21" t="n"/>
-      <c r="C10" s="51" t="s">
-        <v>14</v>
+      <c r="C10" s="51" t="n">
+        <v>0.07000000000000001</v>
       </c>
       <c r="D10" s="143" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="11" spans="1:5">
       <c r="A11" s="21" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B11" s="21" t="n"/>
       <c r="C11" s="51" t="n">
         <v>0.21</v>
       </c>
       <c r="D11" s="143" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="12" spans="1:5">
       <c r="A12" s="21" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B12" s="21" t="n"/>
-      <c r="C12" s="145" t="s">
-        <v>19</v>
-      </c>
+      <c r="C12" s="145" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="14" spans="1:5">
       <c r="A14" s="17" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B14" s="17" t="n"/>
       <c r="C14" s="18" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D14" s="146" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E14" s="107" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="15" spans="1:5">
       <c r="A15" s="21" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="147" t="s">
-        <v>26</v>
+        <v>18</v>
+      </c>
+      <c r="C15" s="147" t="n">
+        <v>6</v>
       </c>
       <c r="D15" s="148">
         <f>ROUND(C15/(1+$C$10),2)</f>
@@ -1730,13 +1679,13 @@
     </row>
     <row customHeight="1" ht="15" r="16" spans="1:5">
       <c r="A16" s="21" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="147" t="s">
-        <v>29</v>
+        <v>20</v>
+      </c>
+      <c r="C16" s="147" t="n">
+        <v>7</v>
       </c>
       <c r="D16" s="148">
         <f>ROUND(C16/(1+$C$10),2)</f>
@@ -1745,13 +1694,13 @@
     </row>
     <row customHeight="1" ht="15" r="17" spans="1:5">
       <c r="A17" s="21" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="147" t="s">
-        <v>32</v>
+        <v>22</v>
+      </c>
+      <c r="C17" s="147" t="n">
+        <v>9</v>
       </c>
       <c r="D17" s="148">
         <f>ROUND(C17/(1+$C$10),2)</f>
@@ -1760,13 +1709,13 @@
     </row>
     <row customHeight="1" ht="15" r="18" spans="1:5">
       <c r="A18" s="21" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="147" t="s">
-        <v>35</v>
+        <v>24</v>
+      </c>
+      <c r="C18" s="147" t="n">
+        <v>5</v>
       </c>
       <c r="D18" s="148">
         <f>ROUND(C18/(1+$C$10),2)</f>
@@ -1775,7 +1724,7 @@
     </row>
     <row hidden="1" r="19" spans="1:5">
       <c r="A19" s="21" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B19" s="67" t="n"/>
       <c r="C19" s="23" t="n"/>
@@ -1792,17 +1741,17 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="67" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C21" s="23" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="22" spans="1:5">
       <c r="A22" s="25" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B22" s="25" t="n"/>
-      <c r="C22" s="147" t="s">
-        <v>35</v>
+      <c r="C22" s="147" t="n">
+        <v>5</v>
       </c>
       <c r="D22" s="148">
         <f>ROUND(C22/(1+$C$10),2)</f>
@@ -1811,11 +1760,11 @@
     </row>
     <row customHeight="1" ht="15" r="23" spans="1:5">
       <c r="A23" s="25" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B23" s="25" t="n"/>
-      <c r="C23" s="147" t="s">
-        <v>35</v>
+      <c r="C23" s="147" t="n">
+        <v>5</v>
       </c>
       <c r="D23" s="148">
         <f>ROUND(C23/(1+$C$10),2)</f>
@@ -1824,11 +1773,11 @@
     </row>
     <row customHeight="1" ht="15" r="24" spans="1:5">
       <c r="A24" s="25" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B24" s="25" t="n"/>
-      <c r="C24" s="147" t="s">
-        <v>35</v>
+      <c r="C24" s="147" t="n">
+        <v>5</v>
       </c>
       <c r="D24" s="148">
         <f>ROUND(C24/(1+$C$10),2)</f>
@@ -1837,11 +1786,11 @@
     </row>
     <row customHeight="1" ht="15" r="25" spans="1:5">
       <c r="A25" s="25" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B25" s="25" t="n"/>
-      <c r="C25" s="147" t="s">
-        <v>35</v>
+      <c r="C25" s="147" t="n">
+        <v>5</v>
       </c>
       <c r="D25" s="148">
         <f>ROUND(C25/(1+$C$10),2)</f>
@@ -1850,11 +1799,11 @@
     </row>
     <row customHeight="1" ht="15" r="26" spans="1:5">
       <c r="A26" s="25" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B26" s="25" t="n"/>
-      <c r="C26" s="147" t="s">
-        <v>35</v>
+      <c r="C26" s="147" t="n">
+        <v>5</v>
       </c>
       <c r="D26" s="148">
         <f>ROUND(C26/(1+$C$10),2)</f>
@@ -1863,11 +1812,11 @@
     </row>
     <row customHeight="1" ht="15" r="27" spans="1:5">
       <c r="A27" s="25" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B27" s="25" t="n"/>
-      <c r="C27" s="147" t="s">
-        <v>35</v>
+      <c r="C27" s="147" t="n">
+        <v>5</v>
       </c>
       <c r="D27" s="148">
         <f>ROUND(C27/(1+$C$10),2)</f>
@@ -1879,13 +1828,13 @@
     </row>
     <row customHeight="1" ht="15" r="29" spans="1:5">
       <c r="A29" s="21" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="147" t="s">
-        <v>46</v>
+        <v>34</v>
+      </c>
+      <c r="C29" s="147" t="n">
+        <v>4</v>
       </c>
       <c r="D29" s="148">
         <f>ROUND(C29/(1+$C$10),2)</f>
@@ -1894,13 +1843,13 @@
     </row>
     <row customHeight="1" ht="15" r="30" spans="1:5">
       <c r="A30" s="21" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" s="147" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="C30" s="147" t="n">
+        <v>5</v>
       </c>
       <c r="D30" s="148">
         <f>ROUND(C30/(1+$C$10),2)</f>
@@ -1976,7 +1925,7 @@
   <sheetData>
     <row customHeight="1" ht="15.75" r="1" spans="1:40">
       <c r="A1" s="117" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="2" spans="1:40">
@@ -1984,14 +1933,11 @@
         <f>Input!C5</f>
         <v/>
       </c>
-      <c r="F2" t="s">
-        <v>50</v>
-      </c>
       <c r="Q2" s="134" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="AK2" s="134" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="3" spans="1:40">
@@ -2000,45 +1946,45 @@
         <v/>
       </c>
       <c r="Q3" s="136" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="V3" s="135" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="AA3" s="135" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="AF3" s="135" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:40">
       <c r="A4" s="130" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C4" s="29">
         <f>IF(Input!C9="Y","Host","Cash")</f>
         <v/>
       </c>
       <c r="E4" s="128" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="H4" s="97" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="I4" s="97" t="n"/>
       <c r="J4" s="98" t="n"/>
       <c r="K4" s="97" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="L4" s="97" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="M4" s="97" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="N4" s="128" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="Q4" s="53" t="n"/>
       <c r="R4" s="53" t="n"/>
@@ -2059,122 +2005,122 @@
     </row>
     <row r="5" spans="1:40">
       <c r="A5" s="130" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C5" s="133">
         <f>Input!C8</f>
         <v/>
       </c>
       <c r="E5" s="128" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="F5" s="128" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="G5" s="128" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="H5" s="100" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="I5" s="100" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="J5" s="98" t="n"/>
       <c r="K5" s="100" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="L5" s="100" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="M5" s="100" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="N5" s="128" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="O5" s="128" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="Q5" s="135" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="R5" s="135" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="S5" s="135" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="T5" s="135" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="V5" s="135" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="W5" s="135" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="X5" s="135" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="Y5" s="135" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="AA5" s="135" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="AB5" s="135" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="AC5" s="135" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="AD5" s="135" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="AF5" s="135" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="AG5" s="135" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="AH5" s="135" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="AI5" s="135" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="AK5" s="104" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="AL5" s="134" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="AM5" s="134" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="AN5" s="101" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row customHeight="1" ht="14.1" r="6" spans="1:40">
       <c r="A6" s="129" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B6" s="132" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E6" s="47" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F6" s="47" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="G6" s="32">
         <f>E6-F6</f>
@@ -2291,16 +2237,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="7" spans="1:40">
       <c r="C7" s="31" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="47" t="s">
-        <v>50</v>
+        <v>18</v>
+      </c>
+      <c r="E7" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G7" s="32">
         <f>E7-F7</f>
@@ -2417,16 +2363,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="8" spans="1:40">
       <c r="C8" s="31" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="47" t="s">
-        <v>50</v>
+        <v>20</v>
+      </c>
+      <c r="E8" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G8" s="32">
         <f>E8-F8</f>
@@ -2543,16 +2489,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="9" spans="1:40">
       <c r="C9" s="31" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" s="47" t="s">
-        <v>50</v>
+        <v>22</v>
+      </c>
+      <c r="E9" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G9" s="32">
         <f>E9-F9</f>
@@ -2669,19 +2615,19 @@
     </row>
     <row customHeight="1" ht="14.1" r="10" spans="1:40">
       <c r="B10" s="121" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="47" t="s">
-        <v>50</v>
+        <v>24</v>
+      </c>
+      <c r="E10" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G10" s="32">
         <f>E10-F10</f>
@@ -2798,16 +2744,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="11" spans="1:40">
       <c r="C11" s="31" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="47" t="s">
-        <v>50</v>
+        <v>18</v>
+      </c>
+      <c r="E11" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G11" s="32">
         <f>E11-F11</f>
@@ -2924,16 +2870,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="12" spans="1:40">
       <c r="C12" s="31" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" s="47" t="s">
-        <v>50</v>
+        <v>20</v>
+      </c>
+      <c r="E12" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G12" s="32">
         <f>E12-F12</f>
@@ -3050,19 +2996,19 @@
     </row>
     <row customHeight="1" ht="14.1" r="13" spans="1:40">
       <c r="B13" s="132" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="47" t="s">
-        <v>50</v>
+        <v>24</v>
+      </c>
+      <c r="E13" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G13" s="32">
         <f>E13-F13</f>
@@ -3179,16 +3125,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="14" spans="1:40">
       <c r="C14" s="31" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="47" t="s">
-        <v>80</v>
+        <v>18</v>
+      </c>
+      <c r="E14" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G14" s="32">
         <f>E14-F14</f>
@@ -3305,16 +3251,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="15" spans="1:40">
       <c r="C15" s="31" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F15" s="47" t="s">
-        <v>50</v>
+        <v>20</v>
+      </c>
+      <c r="E15" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G15" s="32">
         <f>E15-F15</f>
@@ -3431,19 +3377,19 @@
     </row>
     <row customHeight="1" ht="14.1" r="16" spans="1:40">
       <c r="B16" s="121" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="47" t="s">
-        <v>50</v>
+        <v>24</v>
+      </c>
+      <c r="E16" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G16" s="32">
         <f>E16-F16</f>
@@ -3560,16 +3506,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="17" spans="1:40">
       <c r="C17" s="31" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" s="47" t="s">
-        <v>50</v>
+        <v>18</v>
+      </c>
+      <c r="E17" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G17" s="32">
         <f>E17-F17</f>
@@ -3686,16 +3632,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="18" spans="1:40">
       <c r="C18" s="31" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" s="47" t="s">
-        <v>50</v>
+        <v>22</v>
+      </c>
+      <c r="E18" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G18" s="32">
         <f>E18-F18</f>
@@ -3812,19 +3758,19 @@
     </row>
     <row customHeight="1" ht="14.1" r="19" spans="1:40">
       <c r="B19" s="121" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19" s="47" t="s">
-        <v>50</v>
+        <v>20</v>
+      </c>
+      <c r="E19" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G19" s="32">
         <f>E19-F19</f>
@@ -3941,16 +3887,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="20" spans="1:40">
       <c r="C20" s="31" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F20" s="47" t="s">
-        <v>50</v>
+        <v>22</v>
+      </c>
+      <c r="E20" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G20" s="32">
         <f>E20-F20</f>
@@ -4067,19 +4013,19 @@
     </row>
     <row customHeight="1" ht="14.1" r="21" spans="1:40">
       <c r="B21" s="132" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F21" s="47" t="s">
-        <v>50</v>
+        <v>18</v>
+      </c>
+      <c r="E21" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G21" s="32">
         <f>E21-F21</f>
@@ -4196,16 +4142,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="22" spans="1:40">
       <c r="C22" s="31" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="47" t="s">
-        <v>50</v>
+        <v>20</v>
+      </c>
+      <c r="E22" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G22" s="32">
         <f>E22-F22</f>
@@ -4322,19 +4268,19 @@
     </row>
     <row customHeight="1" ht="14.1" r="23" spans="1:40">
       <c r="B23" s="132" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" s="47" t="s">
-        <v>50</v>
+        <v>18</v>
+      </c>
+      <c r="E23" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G23" s="32">
         <f>E23-F23</f>
@@ -4451,16 +4397,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="24" spans="1:40">
       <c r="C24" s="31" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F24" s="47" t="s">
-        <v>50</v>
+        <v>20</v>
+      </c>
+      <c r="E24" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G24" s="32">
         <f>E24-F24</f>
@@ -4577,19 +4523,19 @@
     </row>
     <row customHeight="1" ht="14.1" r="25" spans="1:40">
       <c r="B25" s="121" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F25" s="47" t="s">
-        <v>50</v>
+        <v>24</v>
+      </c>
+      <c r="E25" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G25" s="32">
         <f>E25-F25</f>
@@ -4706,16 +4652,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="26" spans="1:40">
       <c r="C26" s="31" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E26" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F26" s="47" t="s">
-        <v>50</v>
+        <v>24</v>
+      </c>
+      <c r="E26" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G26" s="32">
         <f>E26-F26</f>
@@ -4832,15 +4778,17 @@
     </row>
     <row customHeight="1" ht="14.1" r="27" spans="1:40">
       <c r="C27" s="31" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E27" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F27" s="47" t="n"/>
+        <v>24</v>
+      </c>
+      <c r="E27" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="47" t="n">
+        <v>0</v>
+      </c>
       <c r="G27" s="32">
         <f>E27-F27</f>
         <v/>
@@ -4956,16 +4904,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="28" spans="1:40">
       <c r="C28" s="31" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="D28" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F28" s="47" t="s">
-        <v>50</v>
+        <v>24</v>
+      </c>
+      <c r="E28" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G28" s="32">
         <f>E28-F28</f>
@@ -5082,19 +5030,19 @@
     </row>
     <row customHeight="1" ht="14.1" r="29" spans="1:40">
       <c r="B29" s="123" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C29" s="105" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="E29" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F29" s="47" t="s">
-        <v>50</v>
+        <v>18</v>
+      </c>
+      <c r="E29" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G29" s="32">
         <f>E29-F29</f>
@@ -5211,16 +5159,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="30" spans="1:40">
       <c r="C30" s="48" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="E30" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F30" s="47" t="s">
-        <v>50</v>
+        <v>22</v>
+      </c>
+      <c r="E30" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G30" s="32">
         <f>E30-F30</f>
@@ -5337,16 +5285,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="31" spans="1:40">
       <c r="C31" s="105" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="E31" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="F31" s="47" t="s">
-        <v>50</v>
+        <v>20</v>
+      </c>
+      <c r="E31" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G31" s="32">
         <f>E31-F31</f>
@@ -5463,16 +5411,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="32" spans="1:40">
       <c r="C32" s="105" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="E32" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F32" s="47" t="s">
-        <v>50</v>
+        <v>22</v>
+      </c>
+      <c r="E32" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G32" s="32">
         <f>E32-F32</f>
@@ -5608,10 +5556,10 @@
       <c r="A34" s="35" t="n"/>
       <c r="B34" s="35" t="n"/>
       <c r="C34" s="44" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="D34" s="44" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E34" s="32">
         <f>Q34</f>
@@ -5686,7 +5634,7 @@
       <c r="B35" s="35" t="n"/>
       <c r="C35" s="35" t="n"/>
       <c r="D35" s="44" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E35" s="32">
         <f>V35</f>
@@ -5745,7 +5693,7 @@
       <c r="B36" s="35" t="n"/>
       <c r="C36" s="35" t="n"/>
       <c r="D36" s="44" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E36" s="32">
         <f>AA36</f>
@@ -5808,7 +5756,7 @@
       <c r="B37" s="35" t="n"/>
       <c r="C37" s="35" t="n"/>
       <c r="D37" s="44" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E37" s="32">
         <f>AF37</f>
@@ -5871,7 +5819,7 @@
       <c r="B38" s="35" t="n"/>
       <c r="C38" s="35" t="n"/>
       <c r="D38" s="44" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="E38" s="32">
         <f>SUM(E34:E37)</f>
@@ -5926,33 +5874,33 @@
       <c r="N39" s="35" t="n"/>
       <c r="O39" s="35" t="n"/>
       <c r="Q39" s="134" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="V39" s="134" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="AK39" s="134" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="AL39" s="134" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row customHeight="1" ht="14.1" r="40" spans="1:40">
       <c r="A40" s="129" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="B40" s="116" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="E40" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="F40" s="50" t="s">
-        <v>50</v>
+        <v>34</v>
+      </c>
+      <c r="E40" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="50" t="n">
+        <v>0</v>
       </c>
       <c r="G40" s="41">
         <f>E40-F40</f>
@@ -6028,16 +5976,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="41" spans="1:40">
       <c r="B41" s="119" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D41" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="E41" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="F41" s="50" t="s">
-        <v>50</v>
+        <v>36</v>
+      </c>
+      <c r="E41" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="50" t="n">
+        <v>0</v>
       </c>
       <c r="G41" s="41">
         <f>E41-F41</f>
@@ -6114,16 +6062,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="42" spans="1:40">
       <c r="B42" s="119" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="D42" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="E42" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="F42" s="50" t="s">
-        <v>50</v>
+        <v>34</v>
+      </c>
+      <c r="E42" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" s="50" t="n">
+        <v>0</v>
       </c>
       <c r="G42" s="41">
         <f>E42-F42</f>
@@ -6200,16 +6148,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="43" spans="1:40">
       <c r="B43" s="119" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="D43" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="E43" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="F43" s="50" t="s">
-        <v>50</v>
+        <v>34</v>
+      </c>
+      <c r="E43" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" s="50" t="n">
+        <v>0</v>
       </c>
       <c r="G43" s="41">
         <f>E43-F43</f>
@@ -6286,16 +6234,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="44" spans="1:40">
       <c r="B44" s="119" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="D44" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="E44" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="F44" s="50" t="s">
-        <v>50</v>
+        <v>34</v>
+      </c>
+      <c r="E44" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" s="50" t="n">
+        <v>0</v>
       </c>
       <c r="G44" s="41">
         <f>E44-F44</f>
@@ -6372,16 +6320,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="45" spans="1:40">
       <c r="B45" s="119" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="D45" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="E45" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="F45" s="50" t="s">
-        <v>50</v>
+        <v>36</v>
+      </c>
+      <c r="E45" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" s="50" t="n">
+        <v>0</v>
       </c>
       <c r="G45" s="41">
         <f>E45-F45</f>
@@ -6458,16 +6406,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="46" spans="1:40">
       <c r="B46" s="119" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="D46" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="E46" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="F46" s="50" t="s">
-        <v>50</v>
+        <v>36</v>
+      </c>
+      <c r="E46" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" s="50" t="n">
+        <v>0</v>
       </c>
       <c r="G46" s="41">
         <f>E46-F46</f>
@@ -6544,16 +6492,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="47" spans="1:40">
       <c r="B47" s="119" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="D47" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="E47" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="F47" s="50" t="s">
-        <v>80</v>
+        <v>34</v>
+      </c>
+      <c r="E47" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" s="50" t="n">
+        <v>0</v>
       </c>
       <c r="G47" s="41">
         <f>E47-F47</f>
@@ -6630,16 +6578,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="48" spans="1:40">
       <c r="B48" s="119" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="D48" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="E48" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="F48" s="50" t="s">
-        <v>50</v>
+        <v>34</v>
+      </c>
+      <c r="E48" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" s="50" t="n">
+        <v>0</v>
       </c>
       <c r="G48" s="41">
         <f>E48-F48</f>
@@ -6716,16 +6664,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="49" spans="1:40">
       <c r="B49" s="119" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="D49" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="E49" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="F49" s="50" t="s">
-        <v>50</v>
+        <v>34</v>
+      </c>
+      <c r="E49" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" s="50" t="n">
+        <v>0</v>
       </c>
       <c r="G49" s="41">
         <f>E49-F49</f>
@@ -6802,16 +6750,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="50" spans="1:40">
       <c r="B50" s="119" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="D50" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="E50" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="F50" s="50" t="s">
-        <v>50</v>
+        <v>34</v>
+      </c>
+      <c r="E50" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" s="50" t="n">
+        <v>0</v>
       </c>
       <c r="G50" s="41">
         <f>E50-F50</f>
@@ -6889,7 +6837,7 @@
     <row customHeight="1" ht="14.1" r="51" spans="1:40">
       <c r="B51" s="126" t="n"/>
       <c r="D51" s="31" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="E51" s="50" t="n"/>
       <c r="F51" s="50" t="n"/>
@@ -6969,7 +6917,7 @@
     <row customHeight="1" ht="14.1" r="52" spans="1:40">
       <c r="B52" s="126" t="n"/>
       <c r="D52" s="31" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="E52" s="50" t="n"/>
       <c r="F52" s="50" t="n"/>
@@ -7067,10 +7015,10 @@
       <c r="A54" s="35" t="n"/>
       <c r="B54" s="35" t="n"/>
       <c r="C54" s="43" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="D54" s="44" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="E54" s="41">
         <f>Q54</f>
@@ -7137,7 +7085,7 @@
       <c r="B55" s="35" t="n"/>
       <c r="C55" s="35" t="n"/>
       <c r="D55" s="44" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E55" s="41">
         <f>V55</f>
@@ -7196,7 +7144,7 @@
       <c r="B56" s="35" t="n"/>
       <c r="C56" s="35" t="n"/>
       <c r="D56" s="44" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="E56" s="41">
         <f>SUM(E54:E55)</f>
@@ -7251,24 +7199,24 @@
       <c r="N57" s="35" t="n"/>
       <c r="O57" s="35" t="n"/>
       <c r="AK57" s="134" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
     </row>
     <row customHeight="1" ht="14.1" r="58" spans="1:40">
       <c r="A58" s="129" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="B58" s="116" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D58" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="E58" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F58" s="47" t="s">
-        <v>50</v>
+        <v>106</v>
+      </c>
+      <c r="E58" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G58" s="32">
         <f>E58-F58</f>
@@ -7325,16 +7273,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="59" spans="1:40">
       <c r="B59" s="116" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D59" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="E59" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F59" s="47" t="s">
-        <v>50</v>
+        <v>106</v>
+      </c>
+      <c r="E59" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F59" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G59" s="32">
         <f>E59-F59</f>
@@ -7391,16 +7339,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="60" spans="1:40">
       <c r="B60" s="116" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D60" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="E60" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F60" s="47" t="s">
-        <v>50</v>
+        <v>106</v>
+      </c>
+      <c r="E60" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F60" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G60" s="32">
         <f>E60-F60</f>
@@ -7457,17 +7405,13 @@
     </row>
     <row customHeight="1" ht="14.1" r="61" spans="1:40">
       <c r="B61" s="116" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D61" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="E61" s="106" t="s">
-        <v>50</v>
-      </c>
-      <c r="F61" s="47" t="s">
-        <v>50</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="E61" s="106" t="n"/>
+      <c r="F61" s="47" t="n"/>
       <c r="G61" s="32">
         <f>E61-F61</f>
         <v/>
@@ -7523,16 +7467,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="62" spans="1:40">
       <c r="B62" s="116" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D62" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="E62" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F62" s="47" t="s">
-        <v>50</v>
+        <v>106</v>
+      </c>
+      <c r="E62" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F62" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G62" s="32">
         <f>E62-F62</f>
@@ -7588,16 +7532,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="63" spans="1:40">
       <c r="B63" s="116" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="D63" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="E63" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F63" s="47" t="s">
-        <v>50</v>
+        <v>106</v>
+      </c>
+      <c r="E63" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F63" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G63" s="32">
         <f>E63-F63</f>
@@ -7673,10 +7617,10 @@
       <c r="A65" s="35" t="n"/>
       <c r="B65" s="35" t="n"/>
       <c r="C65" s="43" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="D65" s="44" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="E65" s="32">
         <f>Q65</f>
@@ -7739,7 +7683,7 @@
       <c r="B66" s="35" t="n"/>
       <c r="C66" s="35" t="n"/>
       <c r="D66" s="44" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="E66" s="32">
         <f>SUM(E65:E65)</f>
@@ -7790,7 +7734,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="68" spans="1:40">
       <c r="A68" s="45" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B68" s="46" t="n"/>
       <c r="C68" s="116">
@@ -7806,28 +7750,28 @@
     </row>
     <row customFormat="1" hidden="1" r="70" s="52" spans="1:40">
       <c r="B70" s="52" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C70" s="52" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row customFormat="1" hidden="1" r="71" s="52" spans="1:40">
       <c r="B71" s="52" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C71" s="52" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row customFormat="1" hidden="1" r="72" s="52" spans="1:40">
       <c r="B72" s="52" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row customFormat="1" hidden="1" r="73" s="52" spans="1:40">
       <c r="B73" s="103" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -7935,7 +7879,7 @@
   <sheetData>
     <row customHeight="1" ht="15.75" r="1" spans="1:15">
       <c r="A1" s="137" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="E1" s="65" t="n"/>
       <c r="F1" s="68" t="n"/>
@@ -7964,18 +7908,18 @@
     <row customHeight="1" ht="6.95" r="4" spans="1:15"/>
     <row r="5" spans="1:15">
       <c r="B5" s="18" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="21" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="B6" s="18">
         <f>ROUND(Point!G34*Point!L34,0)</f>
@@ -7992,7 +7936,7 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="21" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B7" s="18">
         <f>ROUND(Point!G35*Point!L35,0)</f>
@@ -8009,7 +7953,7 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="21" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="B8" s="18">
         <f>ROUND(Point!G36*Point!L36,0)</f>
@@ -8026,7 +7970,7 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="21" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="B9" s="18">
         <f>ROUND(Point!G37*Point!L37,0)</f>
@@ -8043,7 +7987,7 @@
     </row>
     <row customFormat="1" r="10" s="74" spans="1:15">
       <c r="A10" s="70" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="B10" s="71">
         <f>SUM(B6:B9)</f>
@@ -8067,7 +8011,7 @@
     <row customHeight="1" ht="6.95" r="11" spans="1:15"/>
     <row r="12" spans="1:15">
       <c r="A12" s="21" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B12" s="18">
         <f>ROUND(Point!G54*Point!L54,0)</f>
@@ -8084,7 +8028,7 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="21" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B13" s="18">
         <f>ROUND(Point!G55*Point!L55,0)</f>
@@ -8101,7 +8045,7 @@
     </row>
     <row customFormat="1" r="14" s="74" spans="1:15">
       <c r="A14" s="70" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B14" s="71">
         <f>SUM(B12:B13)</f>
@@ -8125,7 +8069,7 @@
     <row customHeight="1" ht="6.95" r="15" spans="1:15"/>
     <row r="16" spans="1:15">
       <c r="A16" s="21" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="B16" s="18">
         <f>ROUND(Point!G58*Point!L58,0)</f>
@@ -8142,7 +8086,7 @@
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="21" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="B17" s="18">
         <f>ROUND(Point!G59*Point!L59,0)</f>
@@ -8159,7 +8103,7 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="21" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B18" s="18">
         <f>ROUND(Point!G60*Point!L60,0)</f>
@@ -8176,7 +8120,7 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="21" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="B19" s="18">
         <f>ROUND(Point!G61*Point!L61,0)</f>
@@ -8193,7 +8137,7 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" s="21" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="B20" s="18">
         <f>ROUND(Point!G62*Point!L62,0)</f>
@@ -8210,7 +8154,7 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="21" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="B21" s="18">
         <f>ROUND(Point!G63*Point!L63,0)</f>
@@ -8227,7 +8171,7 @@
     </row>
     <row customFormat="1" r="22" s="74" spans="1:15">
       <c r="A22" s="70" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="B22" s="71">
         <f>SUM(B16:B21)</f>
@@ -8251,11 +8195,11 @@
     <row customHeight="1" ht="6.95" r="23" spans="1:15"/>
     <row r="24" spans="1:15">
       <c r="A24" s="75" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="B24" s="76" t="n"/>
       <c r="C24" s="77" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="D24" s="160">
         <f>ROUND(SUM(D10,D14,D22),2)</f>
@@ -8272,7 +8216,7 @@
         <v/>
       </c>
       <c r="C25" s="77" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="D25" s="159">
         <f>IF(Input!C9="Y",ROUND(Summary!D24*B25,2),0)</f>
@@ -8281,14 +8225,14 @@
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="75" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B26" s="80">
         <f>Input!C10</f>
         <v/>
       </c>
       <c r="C26" s="77" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="D26" s="159">
         <f>ROUND(SUM(D24:D25)*B26,2)</f>
@@ -8302,7 +8246,7 @@
       </c>
       <c r="B27" s="76" t="n"/>
       <c r="C27" s="77" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="D27" s="159">
         <f>SUM(D24:D26)</f>
@@ -8311,11 +8255,11 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="75" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B28" s="76" t="n"/>
       <c r="C28" s="77" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D28" s="159">
         <f>Input!C12</f>
@@ -8329,7 +8273,7 @@
       </c>
       <c r="B29" s="76" t="n"/>
       <c r="C29" s="77" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="D29" s="159">
         <f>IF(Input!C9="Y",Summary!D27,0)</f>
@@ -8339,7 +8283,7 @@
     <row r="30" spans="1:15">
       <c r="B30" s="76" t="n"/>
       <c r="C30" s="77" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="D30" s="159">
         <f>D29+D28-D27</f>
@@ -8355,25 +8299,25 @@
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="140" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
     </row>
     <row customHeight="1" ht="6.95" r="34" spans="1:15"/>
     <row r="35" spans="1:15">
       <c r="A35" s="140" t="n"/>
       <c r="B35" s="83" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="C35" s="71" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="D35" s="71" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="1:15">
       <c r="A36" s="21" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="B36" s="158">
         <f>D6</f>
@@ -8390,7 +8334,7 @@
     </row>
     <row r="37" spans="1:15">
       <c r="A37" s="21" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B37" s="158">
         <f>D7</f>
@@ -8407,7 +8351,7 @@
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="21" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="B38" s="158">
         <f>D8</f>
@@ -8424,7 +8368,7 @@
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="21" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="B39" s="158">
         <f>D9</f>
@@ -8441,7 +8385,7 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="70" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="B40" s="160">
         <f>SUM(B36:B39)</f>
@@ -8459,7 +8403,7 @@
     <row customHeight="1" ht="6.95" r="41" spans="1:15"/>
     <row r="42" spans="1:15">
       <c r="A42" s="70" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B42" s="86">
         <f>Input!D19</f>
@@ -8471,7 +8415,7 @@
     <row customHeight="1" ht="6.95" r="43" spans="1:15"/>
     <row r="44" spans="1:15">
       <c r="A44" s="21" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B44" s="158">
         <f>D12</f>
@@ -8488,7 +8432,7 @@
     </row>
     <row r="45" spans="1:15">
       <c r="A45" s="21" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B45" s="158">
         <f>D13</f>
@@ -8505,7 +8449,7 @@
     </row>
     <row r="46" spans="1:15">
       <c r="A46" s="70" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B46" s="160">
         <f>SUM(B44:B45)</f>
@@ -8523,7 +8467,7 @@
     <row customHeight="1" ht="6.95" r="47" spans="1:15"/>
     <row r="48" spans="1:15">
       <c r="A48" s="21" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B48" s="158">
         <f>D22</f>
@@ -8540,7 +8484,7 @@
     </row>
     <row r="49" spans="1:15">
       <c r="A49" s="70" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="B49" s="160">
         <f>SUM(B48:B48)</f>
@@ -8558,7 +8502,7 @@
     <row customHeight="1" ht="6.95" r="50" spans="1:15"/>
     <row r="51" spans="1:15">
       <c r="A51" s="89" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="B51" s="160">
         <f>B40+B46+B49</f>
@@ -8575,7 +8519,7 @@
     </row>
     <row customFormat="1" hidden="1" r="55" s="68" spans="1:15">
       <c r="F55" s="90" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="G55" s="162">
         <f>Input!C12</f>
@@ -8584,7 +8528,7 @@
     </row>
     <row customFormat="1" hidden="1" r="56" s="68" spans="1:15">
       <c r="F56" s="90" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="G56" s="162">
         <f>ROUND(IF(Input!C10=0,0,G55-(G55/(1+Input!C10))),2)</f>
@@ -8593,7 +8537,7 @@
     </row>
     <row customFormat="1" hidden="1" r="57" s="68" spans="1:15">
       <c r="F57" s="90" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="G57" s="162">
         <f>D14</f>
@@ -8602,7 +8546,7 @@
     </row>
     <row customFormat="1" hidden="1" r="58" s="68" spans="1:15">
       <c r="F58" s="90" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="G58" s="162">
         <f>D22</f>
@@ -8611,7 +8555,7 @@
     </row>
     <row customFormat="1" hidden="1" r="59" s="68" spans="1:15">
       <c r="F59" s="90" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="G59" s="162">
         <f>G55-SUM(G56:G58)</f>
@@ -8620,7 +8564,7 @@
     </row>
     <row customFormat="1" hidden="1" r="60" s="68" spans="1:15">
       <c r="F60" s="90" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="G60" s="162">
         <f>G55-SUM(G56:G59)</f>
@@ -8632,7 +8576,7 @@
     </row>
     <row customFormat="1" hidden="1" r="62" s="68" spans="1:15">
       <c r="F62" s="90" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="G62" s="162">
         <f>G59</f>
@@ -8641,7 +8585,7 @@
     </row>
     <row customFormat="1" hidden="1" r="63" s="68" spans="1:15">
       <c r="F63" s="90" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="G63" s="93">
         <f>Point!G38</f>
@@ -8650,7 +8594,7 @@
     </row>
     <row customFormat="1" hidden="1" r="64" s="68" spans="1:15">
       <c r="F64" s="90" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="G64" s="93">
         <f>26.40825/G62*G63</f>
@@ -8660,24 +8604,24 @@
     <row customFormat="1" hidden="1" r="65" s="68" spans="1:15"/>
     <row customFormat="1" hidden="1" r="66" s="68" spans="1:15">
       <c r="G66" s="94" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="H66" s="94" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="I66" s="94" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="K66" s="94" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="N66" s="94" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
     </row>
     <row customFormat="1" hidden="1" r="67" s="68" spans="1:15">
       <c r="F67" s="90" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G67" s="93">
         <f>Point!G34</f>
@@ -8714,7 +8658,7 @@
     </row>
     <row customFormat="1" hidden="1" r="68" s="68" spans="1:15">
       <c r="F68" s="90" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="G68" s="93">
         <f>Point!G35</f>
@@ -8751,7 +8695,7 @@
     </row>
     <row customFormat="1" hidden="1" r="69" s="68" spans="1:15">
       <c r="F69" s="90" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="G69" s="93">
         <f>Point!G36</f>
@@ -8788,7 +8732,7 @@
     </row>
     <row customFormat="1" hidden="1" r="70" s="68" spans="1:15">
       <c r="F70" s="90" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="G70" s="93">
         <f>Point!G37</f>
@@ -8903,14 +8847,14 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="B1" s="2">
         <f>Input!C5</f>
         <v/>
       </c>
       <c r="D1" s="141" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -8923,7 +8867,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="B3" s="2">
         <f>Summary!A25</f>
@@ -8936,7 +8880,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="B4" s="2">
         <f>Input!C6</f>
@@ -8951,22 +8895,22 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B6" s="166">
         <f>Summary!D10</f>
         <v/>
       </c>
       <c r="F6" s="167" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="G6" s="167" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="B7" s="166">
         <f>Summary!D14</f>
@@ -8976,7 +8920,7 @@
         <v>454598</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="F7" s="168">
         <f>G13</f>
@@ -8986,7 +8930,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="B8" s="166">
         <f>Summary!D22</f>
@@ -8996,7 +8940,7 @@
         <v>464691</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="F8" s="168" t="n"/>
       <c r="G8" s="168">
@@ -9011,7 +8955,7 @@
         <v>464692</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="F9" s="168" t="n"/>
       <c r="G9" s="168">
@@ -9024,7 +8968,7 @@
         <v>464693</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="F10" s="168" t="n"/>
       <c r="G10" s="168">
@@ -9034,7 +8978,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="5" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="B11" s="166">
         <f>Summary!C40</f>
@@ -9044,7 +8988,7 @@
         <v>454598</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="F11" s="168" t="n"/>
       <c r="G11" s="168">
@@ -9054,7 +8998,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="5" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="B12" s="166">
         <f>+Summary!C46</f>
@@ -9064,7 +9008,7 @@
         <v>202220</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="F12" s="168" t="n"/>
       <c r="G12" s="168">
@@ -9074,7 +9018,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="5" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B13" s="166">
         <f>+Summary!C49</f>
@@ -9097,20 +9041,20 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="8" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B17" s="9">
         <f>Point!G8</f>
         <v/>
       </c>
       <c r="D17" s="62" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="E17" s="62" t="n"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="8" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="B18" s="9">
         <f>Point!G25</f>
@@ -9127,7 +9071,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="8" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B19" s="9">
         <f>Point!G10</f>
@@ -9144,7 +9088,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="8" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B20" s="9">
         <f>Point!G13</f>
@@ -9161,7 +9105,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="8" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="B21" s="9">
         <f>Point!G16</f>
@@ -9178,7 +9122,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="8" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B22" s="9">
         <f>Point!G6</f>
@@ -9189,7 +9133,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="8" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B23" s="9">
         <f>Point!G11</f>
@@ -9206,7 +9150,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="8" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="B24" s="9">
         <f>Point!G26</f>
@@ -9223,7 +9167,7 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="8" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B25" s="9">
         <f>Point!G12</f>
@@ -9232,7 +9176,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="8" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B26" s="9">
         <f>Point!G9</f>
@@ -9241,7 +9185,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="8" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="B27" s="9">
         <f>Point!G24</f>
@@ -9250,7 +9194,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="8" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B28" s="9">
         <f>Point!G19</f>
@@ -9259,7 +9203,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="8" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B29" s="9">
         <f>Point!G14</f>
@@ -9268,7 +9212,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="8" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="B30" s="9">
         <f>Point!G20</f>
@@ -9277,7 +9221,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="8" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B31" s="9">
         <f>Point!G22</f>
@@ -9286,7 +9230,7 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="8" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B32" s="9">
         <f>Point!G21</f>
@@ -9295,7 +9239,7 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="8" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B33" s="9">
         <f>Point!G17</f>
@@ -9304,7 +9248,7 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="8" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="B34" s="9">
         <f>Point!G18</f>
@@ -9313,7 +9257,7 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="8" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="B35" s="9">
         <f>Point!G27</f>
@@ -9322,7 +9266,7 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="8" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="B36" s="9">
         <f>Point!G23</f>
@@ -9332,7 +9276,7 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="8" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B37" s="9">
         <f>Point!G7</f>
@@ -9341,7 +9285,7 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="8" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B38" s="9">
         <f>Point!G15</f>
@@ -9350,7 +9294,7 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="8" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="B39" s="9">
         <f>Point!G28</f>
@@ -9362,7 +9306,7 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="10" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="B41" s="169">
         <f>Point!G40</f>
@@ -9371,7 +9315,7 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="10" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="B42" s="169">
         <f>Point!G41</f>
@@ -9381,7 +9325,7 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="10" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="B43" s="169">
         <f>Point!G42</f>
@@ -9391,7 +9335,7 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="10" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="B44" s="169">
         <f>Point!G43</f>
@@ -9401,7 +9345,7 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="10" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="B45" s="169">
         <f>Point!G44</f>
@@ -9411,7 +9355,7 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="10" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="B46" s="169">
         <f>Point!G45</f>
@@ -9420,7 +9364,7 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="10" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="B47" s="169">
         <f>Point!G46</f>
@@ -9429,7 +9373,7 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="10" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="B48" s="169">
         <f>Point!G47</f>
@@ -9438,7 +9382,7 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="10" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="B49" s="169">
         <f>Point!G48</f>
@@ -9447,7 +9391,7 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="10" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B50" s="169">
         <f>Point!G49</f>
@@ -9456,7 +9400,7 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="10" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="B51" s="169">
         <f>Point!G50</f>
@@ -9465,7 +9409,7 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="10" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B53" s="9">
         <f>Point!G58</f>
@@ -9474,7 +9418,7 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="10" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B54" s="9">
         <f>Point!G59</f>
@@ -9483,7 +9427,7 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="10" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B55" s="9">
         <f>Point!G60</f>
@@ -9492,7 +9436,7 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="10" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B56" s="9">
         <f>Point!G61</f>
@@ -9501,7 +9445,7 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="10" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B57" s="9">
         <f>Point!G62</f>
@@ -9510,7 +9454,7 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="10" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="B58" s="9">
         <f>Point!G63</f>

</xml_diff>

<commit_message>
modified home page to load PointSheet on Home.state.data rather than redirecting to separate page / added functionality for retrieving documents from database / delete document functionality not implemented
</commit_message>
<xml_diff>
--- a/client/test.xlsx
+++ b/client/test.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="199">
   <si>
     <t>Greenville Convention Center - Alcohol Point Sheets</t>
   </si>
@@ -36,33 +36,54 @@
     <t>Event Number and Name:</t>
   </si>
   <si>
+    <t>Art Exhibit</t>
+  </si>
+  <si>
     <t>Date of Function</t>
   </si>
   <si>
+    <t>12/20/2018</t>
+  </si>
+  <si>
     <t>Bartender(s):</t>
   </si>
   <si>
+    <t xml:space="preserve">Taylor Mosier </t>
+  </si>
+  <si>
     <t>Room:</t>
   </si>
   <si>
+    <t>Main Bar</t>
+  </si>
+  <si>
     <t>Host Bar (Y/N)</t>
   </si>
   <si>
+    <t>n</t>
+  </si>
+  <si>
     <t>Sales Tax Percentage</t>
   </si>
   <si>
+    <t>7%</t>
+  </si>
+  <si>
     <t>7.00% is default</t>
   </si>
   <si>
     <t>Service Charge Percentage</t>
   </si>
   <si>
-    <t>20.00% is default</t>
+    <t>21%</t>
   </si>
   <si>
     <t>If Cash Bar - Actual Cash Collected:</t>
   </si>
   <si>
+    <t>$1400.00</t>
+  </si>
+  <si>
     <t>PRICES (INCLUDING TAX)</t>
   </si>
   <si>
@@ -81,24 +102,36 @@
     <t>Call</t>
   </si>
   <si>
+    <t>$6.00</t>
+  </si>
+  <si>
     <t>Premium Liquor (Prem)</t>
   </si>
   <si>
     <t>Prem</t>
   </si>
   <si>
+    <t>$7.00</t>
+  </si>
+  <si>
     <t>Top Shelf Premium Liquor (Top)</t>
   </si>
   <si>
     <t>Top</t>
   </si>
   <si>
+    <t>$9.00</t>
+  </si>
+  <si>
     <t>Well Liquor (Top)</t>
   </si>
   <si>
     <t>Well</t>
   </si>
   <si>
+    <t>$5.00</t>
+  </si>
+  <si>
     <t>Number of oz per shot (Calculated/Default)</t>
   </si>
   <si>
@@ -129,6 +162,9 @@
     <t>Dom</t>
   </si>
   <si>
+    <t>$4.00</t>
+  </si>
+  <si>
     <t>Imported Beer</t>
   </si>
   <si>
@@ -195,27 +231,39 @@
     <t>Aristocrat Vodka</t>
   </si>
   <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>Smirnoff</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Absolut</t>
+  </si>
+  <si>
+    <t>Ciroc</t>
+  </si>
+  <si>
+    <t>Rum</t>
+  </si>
+  <si>
+    <t>Aristocrat Rum</t>
+  </si>
+  <si>
+    <t>Bacardi Light</t>
+  </si>
+  <si>
     <t>3</t>
   </si>
   <si>
-    <t>Smirnoff</t>
-  </si>
-  <si>
-    <t>Absolut</t>
-  </si>
-  <si>
-    <t>Ciroc</t>
-  </si>
-  <si>
-    <t>Rum</t>
-  </si>
-  <si>
-    <t>Aristocrat Rum</t>
-  </si>
-  <si>
-    <t>Bacardi Light</t>
-  </si>
-  <si>
     <t>Captain Morgan</t>
   </si>
   <si>
@@ -237,12 +285,21 @@
     <t>Aristocrat Tequila</t>
   </si>
   <si>
+    <t>1.2</t>
+  </si>
+  <si>
     <t>Jose Cuervo Gold</t>
   </si>
   <si>
+    <t>.6</t>
+  </si>
+  <si>
     <t>Patron</t>
   </si>
   <si>
+    <t>.8</t>
+  </si>
+  <si>
     <t>Scotch</t>
   </si>
   <si>
@@ -252,15 +309,27 @@
     <t>Hennessey</t>
   </si>
   <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
     <t>Bourbon</t>
   </si>
   <si>
     <t>Jim Beam</t>
   </si>
   <si>
+    <t>1.6</t>
+  </si>
+  <si>
     <t>Jack Daniels</t>
   </si>
   <si>
+    <t>.3</t>
+  </si>
+  <si>
     <t>Whisky</t>
   </si>
   <si>
@@ -276,9 +345,15 @@
     <t>Amaretto</t>
   </si>
   <si>
+    <t>.5</t>
+  </si>
+  <si>
     <t>Blue Curacao</t>
   </si>
   <si>
+    <t>.4</t>
+  </si>
+  <si>
     <t>Peach Schnapps</t>
   </si>
   <si>
@@ -291,6 +366,9 @@
     <t>Fireball</t>
   </si>
   <si>
+    <t>.2</t>
+  </si>
+  <si>
     <t>Johnnie Walker Black</t>
   </si>
   <si>
@@ -312,6 +390,12 @@
     <t>Bud Light</t>
   </si>
   <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
     <t>Bud Light Platinum</t>
   </si>
   <si>
@@ -321,19 +405,40 @@
     <t>Budwiser</t>
   </si>
   <si>
+    <t>12</t>
+  </si>
+  <si>
     <t>Coors Light</t>
   </si>
   <si>
+    <t>11</t>
+  </si>
+  <si>
     <t>Corona</t>
   </si>
   <si>
+    <t>48</t>
+  </si>
+  <si>
     <t>Heineken</t>
   </si>
   <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
     <t>Michelob Ultra</t>
   </si>
   <si>
+    <t>8</t>
+  </si>
+  <si>
     <t>Miller Lite</t>
+  </si>
+  <si>
+    <t>18</t>
   </si>
   <si>
     <t>Natural Light</t>
@@ -1586,91 +1691,103 @@
         <v>3</v>
       </c>
       <c r="B5" s="21" t="n"/>
-      <c r="C5" s="112" t="n"/>
+      <c r="C5" s="112" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="6" spans="1:5">
       <c r="A6" s="21" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="21" t="n"/>
-      <c r="C6" s="144" t="n"/>
+      <c r="C6" s="144" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="7" spans="1:5">
       <c r="A7" s="21" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7" s="21" t="n"/>
-      <c r="C7" s="112" t="n"/>
+      <c r="C7" s="112" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="8" spans="1:5">
       <c r="A8" s="21" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B8" s="21" t="n"/>
-      <c r="C8" s="112" t="n"/>
+      <c r="C8" s="112" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="9" spans="1:5">
       <c r="A9" s="21" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B9" s="21" t="n"/>
-      <c r="C9" s="112" t="n"/>
+      <c r="C9" s="112" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="10" spans="1:5">
       <c r="A10" s="21" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B10" s="21" t="n"/>
-      <c r="C10" s="51" t="n">
-        <v>0.07000000000000001</v>
+      <c r="C10" s="51" t="s">
+        <v>14</v>
       </c>
       <c r="D10" s="143" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="11" spans="1:5">
       <c r="A11" s="21" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B11" s="21" t="n"/>
       <c r="C11" s="51" t="n">
         <v>0.21</v>
       </c>
       <c r="D11" s="143" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="12" spans="1:5">
       <c r="A12" s="21" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B12" s="21" t="n"/>
-      <c r="C12" s="145" t="n"/>
+      <c r="C12" s="145" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="14" spans="1:5">
       <c r="A14" s="17" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B14" s="17" t="n"/>
       <c r="C14" s="18" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D14" s="146" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E14" s="107" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="15" spans="1:5">
       <c r="A15" s="21" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="147" t="n">
-        <v>6</v>
+        <v>25</v>
+      </c>
+      <c r="C15" s="147" t="s">
+        <v>26</v>
       </c>
       <c r="D15" s="148">
         <f>ROUND(C15/(1+$C$10),2)</f>
@@ -1679,13 +1796,13 @@
     </row>
     <row customHeight="1" ht="15" r="16" spans="1:5">
       <c r="A16" s="21" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="147" t="n">
-        <v>7</v>
+        <v>28</v>
+      </c>
+      <c r="C16" s="147" t="s">
+        <v>29</v>
       </c>
       <c r="D16" s="148">
         <f>ROUND(C16/(1+$C$10),2)</f>
@@ -1694,13 +1811,13 @@
     </row>
     <row customHeight="1" ht="15" r="17" spans="1:5">
       <c r="A17" s="21" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="147" t="n">
-        <v>9</v>
+        <v>31</v>
+      </c>
+      <c r="C17" s="147" t="s">
+        <v>32</v>
       </c>
       <c r="D17" s="148">
         <f>ROUND(C17/(1+$C$10),2)</f>
@@ -1709,13 +1826,13 @@
     </row>
     <row customHeight="1" ht="15" r="18" spans="1:5">
       <c r="A18" s="21" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="147" t="n">
-        <v>5</v>
+        <v>34</v>
+      </c>
+      <c r="C18" s="147" t="s">
+        <v>35</v>
       </c>
       <c r="D18" s="148">
         <f>ROUND(C18/(1+$C$10),2)</f>
@@ -1724,7 +1841,7 @@
     </row>
     <row hidden="1" r="19" spans="1:5">
       <c r="A19" s="21" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B19" s="67" t="n"/>
       <c r="C19" s="23" t="n"/>
@@ -1741,17 +1858,17 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="67" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C21" s="23" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="22" spans="1:5">
       <c r="A22" s="25" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B22" s="25" t="n"/>
-      <c r="C22" s="147" t="n">
-        <v>5</v>
+      <c r="C22" s="147" t="s">
+        <v>35</v>
       </c>
       <c r="D22" s="148">
         <f>ROUND(C22/(1+$C$10),2)</f>
@@ -1760,11 +1877,11 @@
     </row>
     <row customHeight="1" ht="15" r="23" spans="1:5">
       <c r="A23" s="25" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B23" s="25" t="n"/>
-      <c r="C23" s="147" t="n">
-        <v>5</v>
+      <c r="C23" s="147" t="s">
+        <v>35</v>
       </c>
       <c r="D23" s="148">
         <f>ROUND(C23/(1+$C$10),2)</f>
@@ -1773,11 +1890,11 @@
     </row>
     <row customHeight="1" ht="15" r="24" spans="1:5">
       <c r="A24" s="25" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B24" s="25" t="n"/>
-      <c r="C24" s="147" t="n">
-        <v>5</v>
+      <c r="C24" s="147" t="s">
+        <v>35</v>
       </c>
       <c r="D24" s="148">
         <f>ROUND(C24/(1+$C$10),2)</f>
@@ -1786,11 +1903,11 @@
     </row>
     <row customHeight="1" ht="15" r="25" spans="1:5">
       <c r="A25" s="25" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B25" s="25" t="n"/>
-      <c r="C25" s="147" t="n">
-        <v>5</v>
+      <c r="C25" s="147" t="s">
+        <v>35</v>
       </c>
       <c r="D25" s="148">
         <f>ROUND(C25/(1+$C$10),2)</f>
@@ -1799,11 +1916,11 @@
     </row>
     <row customHeight="1" ht="15" r="26" spans="1:5">
       <c r="A26" s="25" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="B26" s="25" t="n"/>
-      <c r="C26" s="147" t="n">
-        <v>5</v>
+      <c r="C26" s="147" t="s">
+        <v>35</v>
       </c>
       <c r="D26" s="148">
         <f>ROUND(C26/(1+$C$10),2)</f>
@@ -1812,11 +1929,11 @@
     </row>
     <row customHeight="1" ht="15" r="27" spans="1:5">
       <c r="A27" s="25" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B27" s="25" t="n"/>
-      <c r="C27" s="147" t="n">
-        <v>5</v>
+      <c r="C27" s="147" t="s">
+        <v>35</v>
       </c>
       <c r="D27" s="148">
         <f>ROUND(C27/(1+$C$10),2)</f>
@@ -1828,13 +1945,13 @@
     </row>
     <row customHeight="1" ht="15" r="29" spans="1:5">
       <c r="A29" s="21" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="147" t="n">
-        <v>4</v>
+        <v>45</v>
+      </c>
+      <c r="C29" s="147" t="s">
+        <v>46</v>
       </c>
       <c r="D29" s="148">
         <f>ROUND(C29/(1+$C$10),2)</f>
@@ -1843,13 +1960,13 @@
     </row>
     <row customHeight="1" ht="15" r="30" spans="1:5">
       <c r="A30" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="147" t="s">
         <v>35</v>
-      </c>
-      <c r="B30" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="147" t="n">
-        <v>5</v>
       </c>
       <c r="D30" s="148">
         <f>ROUND(C30/(1+$C$10),2)</f>
@@ -1925,7 +2042,7 @@
   <sheetData>
     <row customHeight="1" ht="15.75" r="1" spans="1:40">
       <c r="A1" s="117" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="2" spans="1:40">
@@ -1934,10 +2051,10 @@
         <v/>
       </c>
       <c r="Q2" s="134" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="AK2" s="134" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="3" spans="1:40">
@@ -1946,45 +2063,45 @@
         <v/>
       </c>
       <c r="Q3" s="136" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="V3" s="135" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="AA3" s="135" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="AF3" s="135" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:40">
       <c r="A4" s="130" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C4" s="29">
         <f>IF(Input!C9="Y","Host","Cash")</f>
         <v/>
       </c>
       <c r="E4" s="128" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="H4" s="97" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="I4" s="97" t="n"/>
       <c r="J4" s="98" t="n"/>
       <c r="K4" s="97" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="L4" s="97" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="M4" s="97" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="N4" s="128" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="Q4" s="53" t="n"/>
       <c r="R4" s="53" t="n"/>
@@ -2005,122 +2122,122 @@
     </row>
     <row r="5" spans="1:40">
       <c r="A5" s="130" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C5" s="133">
         <f>Input!C8</f>
         <v/>
       </c>
       <c r="E5" s="128" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="F5" s="128" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="G5" s="128" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="H5" s="100" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="I5" s="100" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="J5" s="98" t="n"/>
       <c r="K5" s="100" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="L5" s="100" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="M5" s="100" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="N5" s="128" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="O5" s="128" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="Q5" s="135" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="R5" s="135" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="S5" s="135" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="T5" s="135" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="V5" s="135" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="W5" s="135" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="X5" s="135" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="Y5" s="135" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="AA5" s="135" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="AB5" s="135" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="AC5" s="135" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="AD5" s="135" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="AF5" s="135" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="AG5" s="135" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="AH5" s="135" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="AI5" s="135" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="AK5" s="104" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="AL5" s="134" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="AM5" s="134" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="AN5" s="101" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row customHeight="1" ht="14.1" r="6" spans="1:40">
       <c r="A6" s="129" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B6" s="132" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E6" s="47" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="F6" s="47" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="G6" s="32">
         <f>E6-F6</f>
@@ -2237,16 +2354,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="7" spans="1:40">
       <c r="C7" s="31" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="47" t="n">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="E7" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="47" t="s">
+        <v>73</v>
       </c>
       <c r="G7" s="32">
         <f>E7-F7</f>
@@ -2363,16 +2480,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="8" spans="1:40">
       <c r="C8" s="31" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="47" t="n">
-        <v>0</v>
+        <v>28</v>
+      </c>
+      <c r="E8" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="47" t="s">
+        <v>73</v>
       </c>
       <c r="G8" s="32">
         <f>E8-F8</f>
@@ -2489,10 +2606,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="9" spans="1:40">
       <c r="C9" s="31" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="E9" s="47" t="n">
         <v>0</v>
@@ -2615,13 +2732,13 @@
     </row>
     <row customHeight="1" ht="14.1" r="10" spans="1:40">
       <c r="B10" s="121" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E10" s="47" t="n">
         <v>0</v>
@@ -2744,16 +2861,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="11" spans="1:40">
       <c r="C11" s="31" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="47" t="n">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="E11" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="47" t="s">
+        <v>72</v>
       </c>
       <c r="G11" s="32">
         <f>E11-F11</f>
@@ -2870,10 +2987,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="12" spans="1:40">
       <c r="C12" s="31" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E12" s="47" t="n">
         <v>0</v>
@@ -2996,13 +3113,13 @@
     </row>
     <row customHeight="1" ht="14.1" r="13" spans="1:40">
       <c r="B13" s="132" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E13" s="47" t="n">
         <v>0</v>
@@ -3125,10 +3242,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="14" spans="1:40">
       <c r="C14" s="31" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E14" s="47" t="n">
         <v>0</v>
@@ -3251,16 +3368,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="15" spans="1:40">
       <c r="C15" s="31" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" s="47" t="n">
-        <v>0</v>
+        <v>28</v>
+      </c>
+      <c r="E15" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="47" t="s">
+        <v>79</v>
       </c>
       <c r="G15" s="32">
         <f>E15-F15</f>
@@ -3377,19 +3494,19 @@
     </row>
     <row customHeight="1" ht="14.1" r="16" spans="1:40">
       <c r="B16" s="121" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" s="47" t="n">
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="E16" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="47" t="s">
+        <v>87</v>
       </c>
       <c r="G16" s="32">
         <f>E16-F16</f>
@@ -3506,16 +3623,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="17" spans="1:40">
       <c r="C17" s="31" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" s="47" t="n">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="E17" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="47" t="s">
+        <v>89</v>
       </c>
       <c r="G17" s="32">
         <f>E17-F17</f>
@@ -3632,16 +3749,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="18" spans="1:40">
       <c r="C18" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" s="47" t="n">
-        <v>0</v>
+      <c r="F18" s="47" t="s">
+        <v>91</v>
       </c>
       <c r="G18" s="32">
         <f>E18-F18</f>
@@ -3758,19 +3875,19 @@
     </row>
     <row customHeight="1" ht="14.1" r="19" spans="1:40">
       <c r="B19" s="121" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="47" t="n">
-        <v>0</v>
+      <c r="F19" s="47" t="s">
+        <v>73</v>
       </c>
       <c r="G19" s="32">
         <f>E19-F19</f>
@@ -3887,16 +4004,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="20" spans="1:40">
       <c r="C20" s="31" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" s="47" t="n">
-        <v>0</v>
+        <v>31</v>
+      </c>
+      <c r="E20" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="F20" s="47" t="s">
+        <v>96</v>
       </c>
       <c r="G20" s="32">
         <f>E20-F20</f>
@@ -4013,19 +4130,19 @@
     </row>
     <row customHeight="1" ht="14.1" r="21" spans="1:40">
       <c r="B21" s="132" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" s="47" t="n">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="E21" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="47" t="s">
+        <v>99</v>
       </c>
       <c r="G21" s="32">
         <f>E21-F21</f>
@@ -4142,16 +4259,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="22" spans="1:40">
       <c r="C22" s="31" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" s="47" t="n">
-        <v>0</v>
+        <v>28</v>
+      </c>
+      <c r="E22" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="F22" s="47" t="s">
+        <v>101</v>
       </c>
       <c r="G22" s="32">
         <f>E22-F22</f>
@@ -4268,19 +4385,19 @@
     </row>
     <row customHeight="1" ht="14.1" r="23" spans="1:40">
       <c r="B23" s="132" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F23" s="47" t="n">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="E23" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" s="47" t="s">
+        <v>73</v>
       </c>
       <c r="G23" s="32">
         <f>E23-F23</f>
@@ -4397,16 +4514,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="24" spans="1:40">
       <c r="C24" s="31" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" s="47" t="n">
-        <v>0</v>
+        <v>28</v>
+      </c>
+      <c r="E24" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="47" t="s">
+        <v>73</v>
       </c>
       <c r="G24" s="32">
         <f>E24-F24</f>
@@ -4523,19 +4640,19 @@
     </row>
     <row customHeight="1" ht="14.1" r="25" spans="1:40">
       <c r="B25" s="121" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="E25" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" s="47" t="n">
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="E25" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25" s="47" t="s">
+        <v>107</v>
       </c>
       <c r="G25" s="32">
         <f>E25-F25</f>
@@ -4652,16 +4769,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="26" spans="1:40">
       <c r="C26" s="31" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" s="47" t="n">
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="E26" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="F26" s="47" t="s">
+        <v>109</v>
       </c>
       <c r="G26" s="32">
         <f>E26-F26</f>
@@ -4778,16 +4895,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="27" spans="1:40">
       <c r="C27" s="31" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" s="47" t="n">
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="E27" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="F27" s="47" t="s">
+        <v>91</v>
       </c>
       <c r="G27" s="32">
         <f>E27-F27</f>
@@ -4904,16 +5021,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="28" spans="1:40">
       <c r="C28" s="31" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="D28" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="E28" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" s="47" t="n">
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="E28" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="F28" s="47" t="s">
+        <v>91</v>
       </c>
       <c r="G28" s="32">
         <f>E28-F28</f>
@@ -5030,19 +5147,19 @@
     </row>
     <row customHeight="1" ht="14.1" r="29" spans="1:40">
       <c r="B29" s="123" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="C29" s="105" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="E29" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" s="47" t="n">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="E29" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="F29" s="47" t="s">
+        <v>114</v>
       </c>
       <c r="G29" s="32">
         <f>E29-F29</f>
@@ -5159,16 +5276,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="30" spans="1:40">
       <c r="C30" s="48" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="E30" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" s="47" t="n">
-        <v>0</v>
+        <v>31</v>
+      </c>
+      <c r="E30" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="F30" s="47" t="s">
+        <v>109</v>
       </c>
       <c r="G30" s="32">
         <f>E30-F30</f>
@@ -5285,16 +5402,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="31" spans="1:40">
       <c r="C31" s="105" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="E31" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" s="47" t="n">
-        <v>0</v>
+        <v>28</v>
+      </c>
+      <c r="E31" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="F31" s="47" t="s">
+        <v>109</v>
       </c>
       <c r="G31" s="32">
         <f>E31-F31</f>
@@ -5411,16 +5528,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="32" spans="1:40">
       <c r="C32" s="105" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="E32" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" s="47" t="n">
-        <v>0</v>
+        <v>31</v>
+      </c>
+      <c r="E32" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="F32" s="47" t="s">
+        <v>87</v>
       </c>
       <c r="G32" s="32">
         <f>E32-F32</f>
@@ -5556,10 +5673,10 @@
       <c r="A34" s="35" t="n"/>
       <c r="B34" s="35" t="n"/>
       <c r="C34" s="44" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="D34" s="44" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E34" s="32">
         <f>Q34</f>
@@ -5634,7 +5751,7 @@
       <c r="B35" s="35" t="n"/>
       <c r="C35" s="35" t="n"/>
       <c r="D35" s="44" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E35" s="32">
         <f>V35</f>
@@ -5693,7 +5810,7 @@
       <c r="B36" s="35" t="n"/>
       <c r="C36" s="35" t="n"/>
       <c r="D36" s="44" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E36" s="32">
         <f>AA36</f>
@@ -5756,7 +5873,7 @@
       <c r="B37" s="35" t="n"/>
       <c r="C37" s="35" t="n"/>
       <c r="D37" s="44" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="E37" s="32">
         <f>AF37</f>
@@ -5819,7 +5936,7 @@
       <c r="B38" s="35" t="n"/>
       <c r="C38" s="35" t="n"/>
       <c r="D38" s="44" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="E38" s="32">
         <f>SUM(E34:E37)</f>
@@ -5874,33 +5991,33 @@
       <c r="N39" s="35" t="n"/>
       <c r="O39" s="35" t="n"/>
       <c r="Q39" s="134" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="V39" s="134" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="AK39" s="134" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="AL39" s="134" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row customHeight="1" ht="14.1" r="40" spans="1:40">
       <c r="A40" s="129" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="B40" s="116" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E40" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" s="50" t="n">
-        <v>0</v>
+        <v>45</v>
+      </c>
+      <c r="E40" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="F40" s="50" t="s">
+        <v>123</v>
       </c>
       <c r="G40" s="41">
         <f>E40-F40</f>
@@ -5976,16 +6093,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="41" spans="1:40">
       <c r="B41" s="119" t="s">
+        <v>124</v>
+      </c>
+      <c r="D41" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="E41" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="D41" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="E41" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" s="50" t="n">
-        <v>0</v>
+      <c r="F41" s="50" t="s">
+        <v>96</v>
       </c>
       <c r="G41" s="41">
         <f>E41-F41</f>
@@ -6062,16 +6179,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="42" spans="1:40">
       <c r="B42" s="119" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="D42" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E42" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="F42" s="50" t="n">
-        <v>0</v>
+        <v>45</v>
+      </c>
+      <c r="E42" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="F42" s="50" t="s">
+        <v>96</v>
       </c>
       <c r="G42" s="41">
         <f>E42-F42</f>
@@ -6148,16 +6265,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="43" spans="1:40">
       <c r="B43" s="119" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="D43" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E43" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="F43" s="50" t="n">
-        <v>0</v>
+        <v>45</v>
+      </c>
+      <c r="E43" s="50" t="s">
+        <v>127</v>
+      </c>
+      <c r="F43" s="50" t="s">
+        <v>69</v>
       </c>
       <c r="G43" s="41">
         <f>E43-F43</f>
@@ -6234,16 +6351,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="44" spans="1:40">
       <c r="B44" s="119" t="s">
-        <v>99</v>
+        <v>128</v>
       </c>
       <c r="D44" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E44" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="F44" s="50" t="n">
-        <v>0</v>
+        <v>45</v>
+      </c>
+      <c r="E44" s="50" t="s">
+        <v>127</v>
+      </c>
+      <c r="F44" s="50" t="s">
+        <v>129</v>
       </c>
       <c r="G44" s="41">
         <f>E44-F44</f>
@@ -6320,16 +6437,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="45" spans="1:40">
       <c r="B45" s="119" t="s">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="D45" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="E45" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="F45" s="50" t="n">
-        <v>0</v>
+        <v>48</v>
+      </c>
+      <c r="E45" s="50" t="s">
+        <v>131</v>
+      </c>
+      <c r="F45" s="50" t="s">
+        <v>72</v>
       </c>
       <c r="G45" s="41">
         <f>E45-F45</f>
@@ -6406,16 +6523,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="46" spans="1:40">
       <c r="B46" s="119" t="s">
-        <v>101</v>
+        <v>132</v>
       </c>
       <c r="D46" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="E46" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="F46" s="50" t="n">
-        <v>0</v>
+        <v>48</v>
+      </c>
+      <c r="E46" s="50" t="s">
+        <v>133</v>
+      </c>
+      <c r="F46" s="50" t="s">
+        <v>134</v>
       </c>
       <c r="G46" s="41">
         <f>E46-F46</f>
@@ -6492,16 +6609,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="47" spans="1:40">
       <c r="B47" s="119" t="s">
-        <v>102</v>
+        <v>135</v>
       </c>
       <c r="D47" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E47" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="F47" s="50" t="n">
-        <v>0</v>
+        <v>45</v>
+      </c>
+      <c r="E47" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="F47" s="50" t="s">
+        <v>136</v>
       </c>
       <c r="G47" s="41">
         <f>E47-F47</f>
@@ -6578,16 +6695,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="48" spans="1:40">
       <c r="B48" s="119" t="s">
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="D48" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E48" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="F48" s="50" t="n">
-        <v>0</v>
+        <v>45</v>
+      </c>
+      <c r="E48" s="50" t="s">
+        <v>138</v>
+      </c>
+      <c r="F48" s="50" t="s">
+        <v>129</v>
       </c>
       <c r="G48" s="41">
         <f>E48-F48</f>
@@ -6664,16 +6781,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="49" spans="1:40">
       <c r="B49" s="119" t="s">
-        <v>104</v>
+        <v>139</v>
       </c>
       <c r="D49" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E49" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="F49" s="50" t="n">
-        <v>0</v>
+        <v>45</v>
+      </c>
+      <c r="E49" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="F49" s="50" t="s">
+        <v>96</v>
       </c>
       <c r="G49" s="41">
         <f>E49-F49</f>
@@ -6750,10 +6867,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="50" spans="1:40">
       <c r="B50" s="119" t="s">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="D50" s="31" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="E50" s="50" t="n">
         <v>0</v>
@@ -6837,7 +6954,7 @@
     <row customHeight="1" ht="14.1" r="51" spans="1:40">
       <c r="B51" s="126" t="n"/>
       <c r="D51" s="31" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="E51" s="50" t="n"/>
       <c r="F51" s="50" t="n"/>
@@ -6917,7 +7034,7 @@
     <row customHeight="1" ht="14.1" r="52" spans="1:40">
       <c r="B52" s="126" t="n"/>
       <c r="D52" s="31" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="E52" s="50" t="n"/>
       <c r="F52" s="50" t="n"/>
@@ -7015,10 +7132,10 @@
       <c r="A54" s="35" t="n"/>
       <c r="B54" s="35" t="n"/>
       <c r="C54" s="43" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="D54" s="44" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="E54" s="41">
         <f>Q54</f>
@@ -7085,7 +7202,7 @@
       <c r="B55" s="35" t="n"/>
       <c r="C55" s="35" t="n"/>
       <c r="D55" s="44" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="E55" s="41">
         <f>V55</f>
@@ -7144,7 +7261,7 @@
       <c r="B56" s="35" t="n"/>
       <c r="C56" s="35" t="n"/>
       <c r="D56" s="44" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="E56" s="41">
         <f>SUM(E54:E55)</f>
@@ -7199,18 +7316,18 @@
       <c r="N57" s="35" t="n"/>
       <c r="O57" s="35" t="n"/>
       <c r="AK57" s="134" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
     </row>
     <row customHeight="1" ht="14.1" r="58" spans="1:40">
       <c r="A58" s="129" t="s">
-        <v>107</v>
+        <v>142</v>
       </c>
       <c r="B58" s="116" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D58" s="44" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
       <c r="E58" s="47" t="n">
         <v>0</v>
@@ -7273,10 +7390,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="59" spans="1:40">
       <c r="B59" s="116" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="D59" s="44" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
       <c r="E59" s="47" t="n">
         <v>0</v>
@@ -7339,10 +7456,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="60" spans="1:40">
       <c r="B60" s="116" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="D60" s="44" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
       <c r="E60" s="47" t="n">
         <v>0</v>
@@ -7405,10 +7522,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="61" spans="1:40">
       <c r="B61" s="116" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D61" s="44" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
       <c r="E61" s="106" t="n"/>
       <c r="F61" s="47" t="n"/>
@@ -7467,10 +7584,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="62" spans="1:40">
       <c r="B62" s="116" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="D62" s="44" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
       <c r="E62" s="47" t="n">
         <v>0</v>
@@ -7532,10 +7649,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="63" spans="1:40">
       <c r="B63" s="116" t="s">
-        <v>108</v>
+        <v>143</v>
       </c>
       <c r="D63" s="44" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
       <c r="E63" s="47" t="n">
         <v>0</v>
@@ -7617,10 +7734,10 @@
       <c r="A65" s="35" t="n"/>
       <c r="B65" s="35" t="n"/>
       <c r="C65" s="43" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="D65" s="44" t="s">
-        <v>106</v>
+        <v>141</v>
       </c>
       <c r="E65" s="32">
         <f>Q65</f>
@@ -7683,7 +7800,7 @@
       <c r="B66" s="35" t="n"/>
       <c r="C66" s="35" t="n"/>
       <c r="D66" s="44" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="E66" s="32">
         <f>SUM(E65:E65)</f>
@@ -7734,7 +7851,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="68" spans="1:40">
       <c r="A68" s="45" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B68" s="46" t="n"/>
       <c r="C68" s="116">
@@ -7750,28 +7867,28 @@
     </row>
     <row customFormat="1" hidden="1" r="70" s="52" spans="1:40">
       <c r="B70" s="52" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C70" s="52" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
     </row>
     <row customFormat="1" hidden="1" r="71" s="52" spans="1:40">
       <c r="B71" s="52" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C71" s="52" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row customFormat="1" hidden="1" r="72" s="52" spans="1:40">
       <c r="B72" s="52" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row customFormat="1" hidden="1" r="73" s="52" spans="1:40">
       <c r="B73" s="103" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -7879,7 +7996,7 @@
   <sheetData>
     <row customHeight="1" ht="15.75" r="1" spans="1:15">
       <c r="A1" s="137" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="E1" s="65" t="n"/>
       <c r="F1" s="68" t="n"/>
@@ -7908,18 +8025,18 @@
     <row customHeight="1" ht="6.95" r="4" spans="1:15"/>
     <row r="5" spans="1:15">
       <c r="B5" s="18" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>110</v>
+        <v>145</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>111</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="21" t="s">
-        <v>112</v>
+        <v>147</v>
       </c>
       <c r="B6" s="18">
         <f>ROUND(Point!G34*Point!L34,0)</f>
@@ -7936,7 +8053,7 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="21" t="s">
-        <v>113</v>
+        <v>148</v>
       </c>
       <c r="B7" s="18">
         <f>ROUND(Point!G35*Point!L35,0)</f>
@@ -7953,7 +8070,7 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="21" t="s">
-        <v>114</v>
+        <v>149</v>
       </c>
       <c r="B8" s="18">
         <f>ROUND(Point!G36*Point!L36,0)</f>
@@ -7970,7 +8087,7 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="21" t="s">
-        <v>115</v>
+        <v>150</v>
       </c>
       <c r="B9" s="18">
         <f>ROUND(Point!G37*Point!L37,0)</f>
@@ -7987,7 +8104,7 @@
     </row>
     <row customFormat="1" r="10" s="74" spans="1:15">
       <c r="A10" s="70" t="s">
-        <v>116</v>
+        <v>151</v>
       </c>
       <c r="B10" s="71">
         <f>SUM(B6:B9)</f>
@@ -8011,7 +8128,7 @@
     <row customHeight="1" ht="6.95" r="11" spans="1:15"/>
     <row r="12" spans="1:15">
       <c r="A12" s="21" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B12" s="18">
         <f>ROUND(Point!G54*Point!L54,0)</f>
@@ -8028,7 +8145,7 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="21" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B13" s="18">
         <f>ROUND(Point!G55*Point!L55,0)</f>
@@ -8045,7 +8162,7 @@
     </row>
     <row customFormat="1" r="14" s="74" spans="1:15">
       <c r="A14" s="70" t="s">
-        <v>117</v>
+        <v>152</v>
       </c>
       <c r="B14" s="71">
         <f>SUM(B12:B13)</f>
@@ -8069,7 +8186,7 @@
     <row customHeight="1" ht="6.95" r="15" spans="1:15"/>
     <row r="16" spans="1:15">
       <c r="A16" s="21" t="s">
-        <v>118</v>
+        <v>153</v>
       </c>
       <c r="B16" s="18">
         <f>ROUND(Point!G58*Point!L58,0)</f>
@@ -8086,7 +8203,7 @@
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="21" t="s">
-        <v>119</v>
+        <v>154</v>
       </c>
       <c r="B17" s="18">
         <f>ROUND(Point!G59*Point!L59,0)</f>
@@ -8103,7 +8220,7 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="21" t="s">
-        <v>120</v>
+        <v>155</v>
       </c>
       <c r="B18" s="18">
         <f>ROUND(Point!G60*Point!L60,0)</f>
@@ -8120,7 +8237,7 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="21" t="s">
-        <v>121</v>
+        <v>156</v>
       </c>
       <c r="B19" s="18">
         <f>ROUND(Point!G61*Point!L61,0)</f>
@@ -8137,7 +8254,7 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" s="21" t="s">
-        <v>122</v>
+        <v>157</v>
       </c>
       <c r="B20" s="18">
         <f>ROUND(Point!G62*Point!L62,0)</f>
@@ -8154,7 +8271,7 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="21" t="s">
-        <v>108</v>
+        <v>143</v>
       </c>
       <c r="B21" s="18">
         <f>ROUND(Point!G63*Point!L63,0)</f>
@@ -8171,7 +8288,7 @@
     </row>
     <row customFormat="1" r="22" s="74" spans="1:15">
       <c r="A22" s="70" t="s">
-        <v>123</v>
+        <v>158</v>
       </c>
       <c r="B22" s="71">
         <f>SUM(B16:B21)</f>
@@ -8195,11 +8312,11 @@
     <row customHeight="1" ht="6.95" r="23" spans="1:15"/>
     <row r="24" spans="1:15">
       <c r="A24" s="75" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="B24" s="76" t="n"/>
       <c r="C24" s="77" t="s">
-        <v>124</v>
+        <v>159</v>
       </c>
       <c r="D24" s="160">
         <f>ROUND(SUM(D10,D14,D22),2)</f>
@@ -8216,7 +8333,7 @@
         <v/>
       </c>
       <c r="C25" s="77" t="s">
-        <v>125</v>
+        <v>160</v>
       </c>
       <c r="D25" s="159">
         <f>IF(Input!C9="Y",ROUND(Summary!D24*B25,2),0)</f>
@@ -8225,14 +8342,14 @@
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="75" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B26" s="80">
         <f>Input!C10</f>
         <v/>
       </c>
       <c r="C26" s="77" t="s">
-        <v>126</v>
+        <v>161</v>
       </c>
       <c r="D26" s="159">
         <f>ROUND(SUM(D24:D25)*B26,2)</f>
@@ -8246,7 +8363,7 @@
       </c>
       <c r="B27" s="76" t="n"/>
       <c r="C27" s="77" t="s">
-        <v>127</v>
+        <v>162</v>
       </c>
       <c r="D27" s="159">
         <f>SUM(D24:D26)</f>
@@ -8255,11 +8372,11 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="75" t="s">
-        <v>128</v>
+        <v>163</v>
       </c>
       <c r="B28" s="76" t="n"/>
       <c r="C28" s="77" t="s">
-        <v>129</v>
+        <v>164</v>
       </c>
       <c r="D28" s="159">
         <f>Input!C12</f>
@@ -8273,7 +8390,7 @@
       </c>
       <c r="B29" s="76" t="n"/>
       <c r="C29" s="77" t="s">
-        <v>130</v>
+        <v>165</v>
       </c>
       <c r="D29" s="159">
         <f>IF(Input!C9="Y",Summary!D27,0)</f>
@@ -8283,7 +8400,7 @@
     <row r="30" spans="1:15">
       <c r="B30" s="76" t="n"/>
       <c r="C30" s="77" t="s">
-        <v>131</v>
+        <v>166</v>
       </c>
       <c r="D30" s="159">
         <f>D29+D28-D27</f>
@@ -8299,25 +8416,25 @@
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="140" t="s">
-        <v>132</v>
+        <v>167</v>
       </c>
     </row>
     <row customHeight="1" ht="6.95" r="34" spans="1:15"/>
     <row r="35" spans="1:15">
       <c r="A35" s="140" t="n"/>
       <c r="B35" s="83" t="s">
-        <v>133</v>
+        <v>168</v>
       </c>
       <c r="C35" s="71" t="s">
-        <v>134</v>
+        <v>169</v>
       </c>
       <c r="D35" s="71" t="s">
-        <v>135</v>
+        <v>170</v>
       </c>
     </row>
     <row r="36" spans="1:15">
       <c r="A36" s="21" t="s">
-        <v>112</v>
+        <v>147</v>
       </c>
       <c r="B36" s="158">
         <f>D6</f>
@@ -8334,7 +8451,7 @@
     </row>
     <row r="37" spans="1:15">
       <c r="A37" s="21" t="s">
-        <v>113</v>
+        <v>148</v>
       </c>
       <c r="B37" s="158">
         <f>D7</f>
@@ -8351,7 +8468,7 @@
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="21" t="s">
-        <v>114</v>
+        <v>149</v>
       </c>
       <c r="B38" s="158">
         <f>D8</f>
@@ -8368,7 +8485,7 @@
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="21" t="s">
-        <v>136</v>
+        <v>171</v>
       </c>
       <c r="B39" s="158">
         <f>D9</f>
@@ -8385,7 +8502,7 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="70" t="s">
-        <v>116</v>
+        <v>151</v>
       </c>
       <c r="B40" s="160">
         <f>SUM(B36:B39)</f>
@@ -8403,7 +8520,7 @@
     <row customHeight="1" ht="6.95" r="41" spans="1:15"/>
     <row r="42" spans="1:15">
       <c r="A42" s="70" t="s">
-        <v>137</v>
+        <v>172</v>
       </c>
       <c r="B42" s="86">
         <f>Input!D19</f>
@@ -8415,7 +8532,7 @@
     <row customHeight="1" ht="6.95" r="43" spans="1:15"/>
     <row r="44" spans="1:15">
       <c r="A44" s="21" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B44" s="158">
         <f>D12</f>
@@ -8432,7 +8549,7 @@
     </row>
     <row r="45" spans="1:15">
       <c r="A45" s="21" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B45" s="158">
         <f>D13</f>
@@ -8449,7 +8566,7 @@
     </row>
     <row r="46" spans="1:15">
       <c r="A46" s="70" t="s">
-        <v>117</v>
+        <v>152</v>
       </c>
       <c r="B46" s="160">
         <f>SUM(B44:B45)</f>
@@ -8467,7 +8584,7 @@
     <row customHeight="1" ht="6.95" r="47" spans="1:15"/>
     <row r="48" spans="1:15">
       <c r="A48" s="21" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B48" s="158">
         <f>D22</f>
@@ -8484,7 +8601,7 @@
     </row>
     <row r="49" spans="1:15">
       <c r="A49" s="70" t="s">
-        <v>138</v>
+        <v>173</v>
       </c>
       <c r="B49" s="160">
         <f>SUM(B48:B48)</f>
@@ -8502,7 +8619,7 @@
     <row customHeight="1" ht="6.95" r="50" spans="1:15"/>
     <row r="51" spans="1:15">
       <c r="A51" s="89" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="B51" s="160">
         <f>B40+B46+B49</f>
@@ -8519,7 +8636,7 @@
     </row>
     <row customFormat="1" hidden="1" r="55" s="68" spans="1:15">
       <c r="F55" s="90" t="s">
-        <v>140</v>
+        <v>175</v>
       </c>
       <c r="G55" s="162">
         <f>Input!C12</f>
@@ -8528,7 +8645,7 @@
     </row>
     <row customFormat="1" hidden="1" r="56" s="68" spans="1:15">
       <c r="F56" s="90" t="s">
-        <v>126</v>
+        <v>161</v>
       </c>
       <c r="G56" s="162">
         <f>ROUND(IF(Input!C10=0,0,G55-(G55/(1+Input!C10))),2)</f>
@@ -8537,7 +8654,7 @@
     </row>
     <row customFormat="1" hidden="1" r="57" s="68" spans="1:15">
       <c r="F57" s="90" t="s">
-        <v>141</v>
+        <v>176</v>
       </c>
       <c r="G57" s="162">
         <f>D14</f>
@@ -8546,7 +8663,7 @@
     </row>
     <row customFormat="1" hidden="1" r="58" s="68" spans="1:15">
       <c r="F58" s="90" t="s">
-        <v>142</v>
+        <v>177</v>
       </c>
       <c r="G58" s="162">
         <f>D22</f>
@@ -8555,7 +8672,7 @@
     </row>
     <row customFormat="1" hidden="1" r="59" s="68" spans="1:15">
       <c r="F59" s="90" t="s">
-        <v>143</v>
+        <v>178</v>
       </c>
       <c r="G59" s="162">
         <f>G55-SUM(G56:G58)</f>
@@ -8564,7 +8681,7 @@
     </row>
     <row customFormat="1" hidden="1" r="60" s="68" spans="1:15">
       <c r="F60" s="90" t="s">
-        <v>144</v>
+        <v>179</v>
       </c>
       <c r="G60" s="162">
         <f>G55-SUM(G56:G59)</f>
@@ -8576,7 +8693,7 @@
     </row>
     <row customFormat="1" hidden="1" r="62" s="68" spans="1:15">
       <c r="F62" s="90" t="s">
-        <v>143</v>
+        <v>178</v>
       </c>
       <c r="G62" s="162">
         <f>G59</f>
@@ -8585,7 +8702,7 @@
     </row>
     <row customFormat="1" hidden="1" r="63" s="68" spans="1:15">
       <c r="F63" s="90" t="s">
-        <v>145</v>
+        <v>180</v>
       </c>
       <c r="G63" s="93">
         <f>Point!G38</f>
@@ -8594,7 +8711,7 @@
     </row>
     <row customFormat="1" hidden="1" r="64" s="68" spans="1:15">
       <c r="F64" s="90" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="G64" s="93">
         <f>26.40825/G62*G63</f>
@@ -8604,24 +8721,24 @@
     <row customFormat="1" hidden="1" r="65" s="68" spans="1:15"/>
     <row customFormat="1" hidden="1" r="66" s="68" spans="1:15">
       <c r="G66" s="94" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="H66" s="94" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="I66" s="94" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="K66" s="94" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="N66" s="94" t="s">
-        <v>148</v>
+        <v>183</v>
       </c>
     </row>
     <row customFormat="1" hidden="1" r="67" s="68" spans="1:15">
       <c r="F67" s="90" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="G67" s="93">
         <f>Point!G34</f>
@@ -8658,7 +8775,7 @@
     </row>
     <row customFormat="1" hidden="1" r="68" s="68" spans="1:15">
       <c r="F68" s="90" t="s">
-        <v>149</v>
+        <v>184</v>
       </c>
       <c r="G68" s="93">
         <f>Point!G35</f>
@@ -8695,7 +8812,7 @@
     </row>
     <row customFormat="1" hidden="1" r="69" s="68" spans="1:15">
       <c r="F69" s="90" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="G69" s="93">
         <f>Point!G36</f>
@@ -8732,7 +8849,7 @@
     </row>
     <row customFormat="1" hidden="1" r="70" s="68" spans="1:15">
       <c r="F70" s="90" t="s">
-        <v>151</v>
+        <v>186</v>
       </c>
       <c r="G70" s="93">
         <f>Point!G37</f>
@@ -8847,14 +8964,14 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>152</v>
+        <v>187</v>
       </c>
       <c r="B1" s="2">
         <f>Input!C5</f>
         <v/>
       </c>
       <c r="D1" s="141" t="s">
-        <v>153</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -8867,7 +8984,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
-        <v>154</v>
+        <v>189</v>
       </c>
       <c r="B3" s="2">
         <f>Summary!A25</f>
@@ -8880,7 +8997,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="B4" s="2">
         <f>Input!C6</f>
@@ -8895,22 +9012,22 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
-        <v>143</v>
+        <v>178</v>
       </c>
       <c r="B6" s="166">
         <f>Summary!D10</f>
         <v/>
       </c>
       <c r="F6" s="167" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
       <c r="G6" s="167" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
-        <v>141</v>
+        <v>176</v>
       </c>
       <c r="B7" s="166">
         <f>Summary!D14</f>
@@ -8920,7 +9037,7 @@
         <v>454598</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>158</v>
+        <v>193</v>
       </c>
       <c r="F7" s="168">
         <f>G13</f>
@@ -8930,7 +9047,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
-        <v>142</v>
+        <v>177</v>
       </c>
       <c r="B8" s="166">
         <f>Summary!D22</f>
@@ -8940,7 +9057,7 @@
         <v>464691</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>143</v>
+        <v>178</v>
       </c>
       <c r="F8" s="168" t="n"/>
       <c r="G8" s="168">
@@ -8955,7 +9072,7 @@
         <v>464692</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>141</v>
+        <v>176</v>
       </c>
       <c r="F9" s="168" t="n"/>
       <c r="G9" s="168">
@@ -8968,7 +9085,7 @@
         <v>464693</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>142</v>
+        <v>177</v>
       </c>
       <c r="F10" s="168" t="n"/>
       <c r="G10" s="168">
@@ -8978,7 +9095,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="5" t="s">
-        <v>159</v>
+        <v>194</v>
       </c>
       <c r="B11" s="166">
         <f>Summary!C40</f>
@@ -8988,7 +9105,7 @@
         <v>454598</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>160</v>
+        <v>195</v>
       </c>
       <c r="F11" s="168" t="n"/>
       <c r="G11" s="168">
@@ -8998,7 +9115,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="5" t="s">
-        <v>161</v>
+        <v>196</v>
       </c>
       <c r="B12" s="166">
         <f>+Summary!C46</f>
@@ -9008,7 +9125,7 @@
         <v>202220</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>126</v>
+        <v>161</v>
       </c>
       <c r="F12" s="168" t="n"/>
       <c r="G12" s="168">
@@ -9018,7 +9135,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="5" t="s">
-        <v>162</v>
+        <v>197</v>
       </c>
       <c r="B13" s="166">
         <f>+Summary!C49</f>
@@ -9041,20 +9158,20 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="8" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="B17" s="9">
         <f>Point!G8</f>
         <v/>
       </c>
       <c r="D17" s="62" t="s">
-        <v>163</v>
+        <v>198</v>
       </c>
       <c r="E17" s="62" t="n"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="8" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="B18" s="9">
         <f>Point!G25</f>
@@ -9071,7 +9188,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="8" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="B19" s="9">
         <f>Point!G10</f>
@@ -9088,7 +9205,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="8" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B20" s="9">
         <f>Point!G13</f>
@@ -9105,7 +9222,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="8" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="B21" s="9">
         <f>Point!G16</f>
@@ -9122,7 +9239,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="8" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="B22" s="9">
         <f>Point!G6</f>
@@ -9133,7 +9250,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="8" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="B23" s="9">
         <f>Point!G11</f>
@@ -9150,7 +9267,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="8" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="B24" s="9">
         <f>Point!G26</f>
@@ -9167,7 +9284,7 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="8" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="B25" s="9">
         <f>Point!G12</f>
@@ -9176,7 +9293,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="8" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B26" s="9">
         <f>Point!G9</f>
@@ -9185,7 +9302,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="8" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="B27" s="9">
         <f>Point!G24</f>
@@ -9194,7 +9311,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="8" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="B28" s="9">
         <f>Point!G19</f>
@@ -9203,7 +9320,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="8" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="B29" s="9">
         <f>Point!G14</f>
@@ -9212,7 +9329,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="8" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="B30" s="9">
         <f>Point!G20</f>
@@ -9221,7 +9338,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="8" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="B31" s="9">
         <f>Point!G22</f>
@@ -9230,7 +9347,7 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="8" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="B32" s="9">
         <f>Point!G21</f>
@@ -9239,7 +9356,7 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="8" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="B33" s="9">
         <f>Point!G17</f>
@@ -9248,7 +9365,7 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="8" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="B34" s="9">
         <f>Point!G18</f>
@@ -9257,7 +9374,7 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="8" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="B35" s="9">
         <f>Point!G27</f>
@@ -9266,7 +9383,7 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="8" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="B36" s="9">
         <f>Point!G23</f>
@@ -9276,7 +9393,7 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="8" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="B37" s="9">
         <f>Point!G7</f>
@@ -9285,7 +9402,7 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="8" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="B38" s="9">
         <f>Point!G15</f>
@@ -9294,7 +9411,7 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="8" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="B39" s="9">
         <f>Point!G28</f>
@@ -9306,7 +9423,7 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="10" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="B41" s="169">
         <f>Point!G40</f>
@@ -9315,7 +9432,7 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="10" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="B42" s="169">
         <f>Point!G41</f>
@@ -9325,7 +9442,7 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="10" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="B43" s="169">
         <f>Point!G42</f>
@@ -9335,7 +9452,7 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="10" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="B44" s="169">
         <f>Point!G43</f>
@@ -9345,7 +9462,7 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="10" t="s">
-        <v>99</v>
+        <v>128</v>
       </c>
       <c r="B45" s="169">
         <f>Point!G44</f>
@@ -9355,7 +9472,7 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="10" t="s">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="B46" s="169">
         <f>Point!G45</f>
@@ -9364,7 +9481,7 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="10" t="s">
-        <v>101</v>
+        <v>132</v>
       </c>
       <c r="B47" s="169">
         <f>Point!G46</f>
@@ -9373,7 +9490,7 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="10" t="s">
-        <v>102</v>
+        <v>135</v>
       </c>
       <c r="B48" s="169">
         <f>Point!G47</f>
@@ -9382,7 +9499,7 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="10" t="s">
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="B49" s="169">
         <f>Point!G48</f>
@@ -9391,7 +9508,7 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="10" t="s">
-        <v>104</v>
+        <v>139</v>
       </c>
       <c r="B50" s="169">
         <f>Point!G49</f>
@@ -9400,7 +9517,7 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="10" t="s">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="B51" s="169">
         <f>Point!G50</f>
@@ -9409,7 +9526,7 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="10" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B53" s="9">
         <f>Point!G58</f>
@@ -9418,7 +9535,7 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="10" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B54" s="9">
         <f>Point!G59</f>
@@ -9427,7 +9544,7 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="10" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B55" s="9">
         <f>Point!G60</f>
@@ -9436,7 +9553,7 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="10" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B56" s="9">
         <f>Point!G61</f>
@@ -9445,7 +9562,7 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="10" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="B57" s="9">
         <f>Point!G62</f>
@@ -9454,7 +9571,7 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="10" t="s">
-        <v>108</v>
+        <v>143</v>
       </c>
       <c r="B58" s="9">
         <f>Point!G63</f>

</xml_diff>

<commit_message>
refactored data strcuture of python info dictionary / Labels now properly formattd
</commit_message>
<xml_diff>
--- a/client/test.xlsx
+++ b/client/test.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="174">
   <si>
     <t>Greenville Convention Center - Alcohol Point Sheets</t>
   </si>
@@ -36,7 +36,7 @@
     <t>Event Number and Name:</t>
   </si>
   <si>
-    <t>hjhjk</t>
+    <t>Tatttt</t>
   </si>
   <si>
     <t>Date of Function</t>
@@ -220,6 +220,12 @@
   </si>
   <si>
     <t>Aristocrat Vodka</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
   <si>
     <t>Smirnoff</t>
@@ -2146,11 +2152,11 @@
       <c r="D6" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="47" t="n">
-        <v>0</v>
+      <c r="E6" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="47" t="s">
+        <v>67</v>
       </c>
       <c r="G6" s="32">
         <f>E6-F6</f>
@@ -2267,7 +2273,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="7" spans="1:40">
       <c r="C7" s="31" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>22</v>
@@ -2393,7 +2399,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="8" spans="1:40">
       <c r="C8" s="31" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>25</v>
@@ -2519,7 +2525,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="9" spans="1:40">
       <c r="C9" s="31" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>28</v>
@@ -2645,10 +2651,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="10" spans="1:40">
       <c r="B10" s="121" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>31</v>
@@ -2774,7 +2780,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="11" spans="1:40">
       <c r="C11" s="31" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>22</v>
@@ -2900,7 +2906,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="12" spans="1:40">
       <c r="C12" s="31" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>25</v>
@@ -3026,10 +3032,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="13" spans="1:40">
       <c r="B13" s="132" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>31</v>
@@ -3155,7 +3161,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="14" spans="1:40">
       <c r="C14" s="31" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>22</v>
@@ -3281,7 +3287,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="15" spans="1:40">
       <c r="C15" s="31" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>25</v>
@@ -3407,10 +3413,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="16" spans="1:40">
       <c r="B16" s="121" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>31</v>
@@ -3536,7 +3542,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="17" spans="1:40">
       <c r="C17" s="31" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>22</v>
@@ -3662,7 +3668,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="18" spans="1:40">
       <c r="C18" s="31" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>28</v>
@@ -3788,10 +3794,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="19" spans="1:40">
       <c r="B19" s="121" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D19" s="31" t="s">
         <v>25</v>
@@ -3917,7 +3923,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="20" spans="1:40">
       <c r="C20" s="31" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D20" s="31" t="s">
         <v>28</v>
@@ -4043,10 +4049,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="21" spans="1:40">
       <c r="B21" s="132" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D21" s="31" t="s">
         <v>22</v>
@@ -4172,7 +4178,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="22" spans="1:40">
       <c r="C22" s="31" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D22" s="31" t="s">
         <v>25</v>
@@ -4298,10 +4304,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="23" spans="1:40">
       <c r="B23" s="132" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D23" s="31" t="s">
         <v>22</v>
@@ -4427,7 +4433,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="24" spans="1:40">
       <c r="C24" s="31" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D24" s="31" t="s">
         <v>25</v>
@@ -4553,10 +4559,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="25" spans="1:40">
       <c r="B25" s="121" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D25" s="31" t="s">
         <v>31</v>
@@ -4682,7 +4688,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="26" spans="1:40">
       <c r="C26" s="31" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D26" s="31" t="s">
         <v>31</v>
@@ -4808,7 +4814,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="27" spans="1:40">
       <c r="C27" s="31" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D27" s="31" t="s">
         <v>31</v>
@@ -4934,7 +4940,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="28" spans="1:40">
       <c r="C28" s="31" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D28" s="31" t="s">
         <v>31</v>
@@ -5060,10 +5066,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="29" spans="1:40">
       <c r="B29" s="123" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C29" s="105" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D29" s="31" t="s">
         <v>22</v>
@@ -5189,7 +5195,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="30" spans="1:40">
       <c r="C30" s="48" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D30" s="31" t="s">
         <v>28</v>
@@ -5315,7 +5321,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="31" spans="1:40">
       <c r="C31" s="105" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D31" s="31" t="s">
         <v>25</v>
@@ -5441,7 +5447,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="32" spans="1:40">
       <c r="C32" s="105" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D32" s="31" t="s">
         <v>28</v>
@@ -5586,7 +5592,7 @@
       <c r="A34" s="35" t="n"/>
       <c r="B34" s="35" t="n"/>
       <c r="C34" s="44" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D34" s="44" t="s">
         <v>31</v>
@@ -5849,7 +5855,7 @@
       <c r="B38" s="35" t="n"/>
       <c r="C38" s="35" t="n"/>
       <c r="D38" s="44" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E38" s="32">
         <f>SUM(E34:E37)</f>
@@ -5918,10 +5924,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="40" spans="1:40">
       <c r="A40" s="129" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B40" s="116" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D40" s="31" t="s">
         <v>42</v>
@@ -6006,7 +6012,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="41" spans="1:40">
       <c r="B41" s="119" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D41" s="31" t="s">
         <v>45</v>
@@ -6092,7 +6098,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="42" spans="1:40">
       <c r="B42" s="119" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D42" s="31" t="s">
         <v>42</v>
@@ -6178,7 +6184,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="43" spans="1:40">
       <c r="B43" s="119" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D43" s="31" t="s">
         <v>42</v>
@@ -6264,7 +6270,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="44" spans="1:40">
       <c r="B44" s="119" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D44" s="31" t="s">
         <v>42</v>
@@ -6350,7 +6356,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="45" spans="1:40">
       <c r="B45" s="119" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D45" s="31" t="s">
         <v>45</v>
@@ -6436,7 +6442,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="46" spans="1:40">
       <c r="B46" s="119" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D46" s="31" t="s">
         <v>45</v>
@@ -6522,7 +6528,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="47" spans="1:40">
       <c r="B47" s="119" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D47" s="31" t="s">
         <v>42</v>
@@ -6608,7 +6614,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="48" spans="1:40">
       <c r="B48" s="119" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D48" s="31" t="s">
         <v>42</v>
@@ -6694,7 +6700,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="49" spans="1:40">
       <c r="B49" s="119" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D49" s="31" t="s">
         <v>42</v>
@@ -6780,7 +6786,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="50" spans="1:40">
       <c r="B50" s="119" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D50" s="31" t="s">
         <v>42</v>
@@ -7045,7 +7051,7 @@
       <c r="A54" s="35" t="n"/>
       <c r="B54" s="35" t="n"/>
       <c r="C54" s="43" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D54" s="44" t="s">
         <v>42</v>
@@ -7174,7 +7180,7 @@
       <c r="B56" s="35" t="n"/>
       <c r="C56" s="35" t="n"/>
       <c r="D56" s="44" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E56" s="41">
         <f>SUM(E54:E55)</f>
@@ -7229,18 +7235,18 @@
       <c r="N57" s="35" t="n"/>
       <c r="O57" s="35" t="n"/>
       <c r="AK57" s="134" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row customHeight="1" ht="14.1" r="58" spans="1:40">
       <c r="A58" s="129" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B58" s="116" t="s">
         <v>35</v>
       </c>
       <c r="D58" s="44" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E58" s="47" t="n">
         <v>0</v>
@@ -7306,7 +7312,7 @@
         <v>36</v>
       </c>
       <c r="D59" s="44" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E59" s="47" t="n">
         <v>0</v>
@@ -7372,7 +7378,7 @@
         <v>37</v>
       </c>
       <c r="D60" s="44" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E60" s="47" t="n">
         <v>0</v>
@@ -7438,7 +7444,7 @@
         <v>38</v>
       </c>
       <c r="D61" s="44" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E61" s="106" t="n"/>
       <c r="F61" s="47" t="n"/>
@@ -7500,7 +7506,7 @@
         <v>39</v>
       </c>
       <c r="D62" s="44" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E62" s="47" t="n">
         <v>0</v>
@@ -7562,10 +7568,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="63" spans="1:40">
       <c r="B63" s="116" t="s">
+        <v>118</v>
+      </c>
+      <c r="D63" s="44" t="s">
         <v>116</v>
-      </c>
-      <c r="D63" s="44" t="s">
-        <v>114</v>
       </c>
       <c r="E63" s="47" t="n">
         <v>0</v>
@@ -7647,10 +7653,10 @@
       <c r="A65" s="35" t="n"/>
       <c r="B65" s="35" t="n"/>
       <c r="C65" s="43" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D65" s="44" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E65" s="32">
         <f>Q65</f>
@@ -7713,7 +7719,7 @@
       <c r="B66" s="35" t="n"/>
       <c r="C66" s="35" t="n"/>
       <c r="D66" s="44" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E66" s="32">
         <f>SUM(E65:E65)</f>
@@ -7909,7 +7915,7 @@
   <sheetData>
     <row customHeight="1" ht="15.75" r="1" spans="1:15">
       <c r="A1" s="137" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E1" s="65" t="n"/>
       <c r="F1" s="68" t="n"/>
@@ -7941,15 +7947,15 @@
         <v>50</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="21" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B6" s="18">
         <f>ROUND(Point!G34*Point!L34,0)</f>
@@ -7966,7 +7972,7 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="21" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B7" s="18">
         <f>ROUND(Point!G35*Point!L35,0)</f>
@@ -7983,7 +7989,7 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="21" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B8" s="18">
         <f>ROUND(Point!G36*Point!L36,0)</f>
@@ -8000,7 +8006,7 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="21" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B9" s="18">
         <f>ROUND(Point!G37*Point!L37,0)</f>
@@ -8017,7 +8023,7 @@
     </row>
     <row customFormat="1" r="10" s="74" spans="1:15">
       <c r="A10" s="70" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B10" s="71">
         <f>SUM(B6:B9)</f>
@@ -8075,7 +8081,7 @@
     </row>
     <row customFormat="1" r="14" s="74" spans="1:15">
       <c r="A14" s="70" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B14" s="71">
         <f>SUM(B12:B13)</f>
@@ -8099,7 +8105,7 @@
     <row customHeight="1" ht="6.95" r="15" spans="1:15"/>
     <row r="16" spans="1:15">
       <c r="A16" s="21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B16" s="18">
         <f>ROUND(Point!G58*Point!L58,0)</f>
@@ -8116,7 +8122,7 @@
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="21" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B17" s="18">
         <f>ROUND(Point!G59*Point!L59,0)</f>
@@ -8133,7 +8139,7 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="21" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B18" s="18">
         <f>ROUND(Point!G60*Point!L60,0)</f>
@@ -8150,7 +8156,7 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="21" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B19" s="18">
         <f>ROUND(Point!G61*Point!L61,0)</f>
@@ -8167,7 +8173,7 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" s="21" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B20" s="18">
         <f>ROUND(Point!G62*Point!L62,0)</f>
@@ -8184,7 +8190,7 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="21" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B21" s="18">
         <f>ROUND(Point!G63*Point!L63,0)</f>
@@ -8201,7 +8207,7 @@
     </row>
     <row customFormat="1" r="22" s="74" spans="1:15">
       <c r="A22" s="70" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B22" s="71">
         <f>SUM(B16:B21)</f>
@@ -8229,7 +8235,7 @@
       </c>
       <c r="B24" s="76" t="n"/>
       <c r="C24" s="77" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D24" s="160">
         <f>ROUND(SUM(D10,D14,D22),2)</f>
@@ -8246,7 +8252,7 @@
         <v/>
       </c>
       <c r="C25" s="77" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D25" s="159">
         <f>IF(Input!C9="Y",ROUND(Summary!D24*B25,2),0)</f>
@@ -8262,7 +8268,7 @@
         <v/>
       </c>
       <c r="C26" s="77" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D26" s="159">
         <f>ROUND(SUM(D24:D25)*B26,2)</f>
@@ -8276,7 +8282,7 @@
       </c>
       <c r="B27" s="76" t="n"/>
       <c r="C27" s="77" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D27" s="159">
         <f>SUM(D24:D26)</f>
@@ -8285,11 +8291,11 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="75" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B28" s="76" t="n"/>
       <c r="C28" s="77" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D28" s="159">
         <f>Input!C12</f>
@@ -8303,7 +8309,7 @@
       </c>
       <c r="B29" s="76" t="n"/>
       <c r="C29" s="77" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D29" s="159">
         <f>IF(Input!C9="Y",Summary!D27,0)</f>
@@ -8313,7 +8319,7 @@
     <row r="30" spans="1:15">
       <c r="B30" s="76" t="n"/>
       <c r="C30" s="77" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D30" s="159">
         <f>D29+D28-D27</f>
@@ -8329,25 +8335,25 @@
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="140" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row customHeight="1" ht="6.95" r="34" spans="1:15"/>
     <row r="35" spans="1:15">
       <c r="A35" s="140" t="n"/>
       <c r="B35" s="83" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C35" s="71" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D35" s="71" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:15">
       <c r="A36" s="21" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B36" s="158">
         <f>D6</f>
@@ -8364,7 +8370,7 @@
     </row>
     <row r="37" spans="1:15">
       <c r="A37" s="21" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B37" s="158">
         <f>D7</f>
@@ -8381,7 +8387,7 @@
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="21" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B38" s="158">
         <f>D8</f>
@@ -8398,7 +8404,7 @@
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="21" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B39" s="158">
         <f>D9</f>
@@ -8415,7 +8421,7 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="70" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B40" s="160">
         <f>SUM(B36:B39)</f>
@@ -8433,7 +8439,7 @@
     <row customHeight="1" ht="6.95" r="41" spans="1:15"/>
     <row r="42" spans="1:15">
       <c r="A42" s="70" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B42" s="86">
         <f>Input!D19</f>
@@ -8479,7 +8485,7 @@
     </row>
     <row r="46" spans="1:15">
       <c r="A46" s="70" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B46" s="160">
         <f>SUM(B44:B45)</f>
@@ -8514,7 +8520,7 @@
     </row>
     <row r="49" spans="1:15">
       <c r="A49" s="70" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B49" s="160">
         <f>SUM(B48:B48)</f>
@@ -8532,7 +8538,7 @@
     <row customHeight="1" ht="6.95" r="50" spans="1:15"/>
     <row r="51" spans="1:15">
       <c r="A51" s="89" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B51" s="160">
         <f>B40+B46+B49</f>
@@ -8549,7 +8555,7 @@
     </row>
     <row customFormat="1" hidden="1" r="55" s="68" spans="1:15">
       <c r="F55" s="90" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="G55" s="162">
         <f>Input!C12</f>
@@ -8558,7 +8564,7 @@
     </row>
     <row customFormat="1" hidden="1" r="56" s="68" spans="1:15">
       <c r="F56" s="90" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G56" s="162">
         <f>ROUND(IF(Input!C10=0,0,G55-(G55/(1+Input!C10))),2)</f>
@@ -8567,7 +8573,7 @@
     </row>
     <row customFormat="1" hidden="1" r="57" s="68" spans="1:15">
       <c r="F57" s="90" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G57" s="162">
         <f>D14</f>
@@ -8576,7 +8582,7 @@
     </row>
     <row customFormat="1" hidden="1" r="58" s="68" spans="1:15">
       <c r="F58" s="90" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="G58" s="162">
         <f>D22</f>
@@ -8585,7 +8591,7 @@
     </row>
     <row customFormat="1" hidden="1" r="59" s="68" spans="1:15">
       <c r="F59" s="90" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G59" s="162">
         <f>G55-SUM(G56:G58)</f>
@@ -8594,7 +8600,7 @@
     </row>
     <row customFormat="1" hidden="1" r="60" s="68" spans="1:15">
       <c r="F60" s="90" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="G60" s="162">
         <f>G55-SUM(G56:G59)</f>
@@ -8606,7 +8612,7 @@
     </row>
     <row customFormat="1" hidden="1" r="62" s="68" spans="1:15">
       <c r="F62" s="90" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G62" s="162">
         <f>G59</f>
@@ -8615,7 +8621,7 @@
     </row>
     <row customFormat="1" hidden="1" r="63" s="68" spans="1:15">
       <c r="F63" s="90" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G63" s="93">
         <f>Point!G38</f>
@@ -8624,7 +8630,7 @@
     </row>
     <row customFormat="1" hidden="1" r="64" s="68" spans="1:15">
       <c r="F64" s="90" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G64" s="93">
         <f>26.40825/G62*G63</f>
@@ -8640,13 +8646,13 @@
         <v>51</v>
       </c>
       <c r="I66" s="94" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="K66" s="94" t="s">
         <v>58</v>
       </c>
       <c r="N66" s="94" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row customFormat="1" hidden="1" r="67" s="68" spans="1:15">
@@ -8688,7 +8694,7 @@
     </row>
     <row customFormat="1" hidden="1" r="68" s="68" spans="1:15">
       <c r="F68" s="90" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="G68" s="93">
         <f>Point!G35</f>
@@ -8725,7 +8731,7 @@
     </row>
     <row customFormat="1" hidden="1" r="69" s="68" spans="1:15">
       <c r="F69" s="90" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G69" s="93">
         <f>Point!G36</f>
@@ -8762,7 +8768,7 @@
     </row>
     <row customFormat="1" hidden="1" r="70" s="68" spans="1:15">
       <c r="F70" s="90" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="G70" s="93">
         <f>Point!G37</f>
@@ -8877,14 +8883,14 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B1" s="2">
         <f>Input!C5</f>
         <v/>
       </c>
       <c r="D1" s="141" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -8897,7 +8903,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B3" s="2">
         <f>Summary!A25</f>
@@ -8910,7 +8916,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B4" s="2">
         <f>Input!C6</f>
@@ -8925,22 +8931,22 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B6" s="166">
         <f>Summary!D10</f>
         <v/>
       </c>
       <c r="F6" s="167" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="G6" s="167" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B7" s="166">
         <f>Summary!D14</f>
@@ -8950,7 +8956,7 @@
         <v>454598</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F7" s="168">
         <f>G13</f>
@@ -8960,7 +8966,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B8" s="166">
         <f>Summary!D22</f>
@@ -8970,7 +8976,7 @@
         <v>464691</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F8" s="168" t="n"/>
       <c r="G8" s="168">
@@ -8985,7 +8991,7 @@
         <v>464692</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F9" s="168" t="n"/>
       <c r="G9" s="168">
@@ -8998,7 +9004,7 @@
         <v>464693</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F10" s="168" t="n"/>
       <c r="G10" s="168">
@@ -9008,7 +9014,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="5" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B11" s="166">
         <f>Summary!C40</f>
@@ -9018,7 +9024,7 @@
         <v>454598</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F11" s="168" t="n"/>
       <c r="G11" s="168">
@@ -9028,7 +9034,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="5" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B12" s="166">
         <f>+Summary!C46</f>
@@ -9038,7 +9044,7 @@
         <v>202220</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F12" s="168" t="n"/>
       <c r="G12" s="168">
@@ -9048,7 +9054,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="5" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B13" s="166">
         <f>+Summary!C49</f>
@@ -9071,20 +9077,20 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B17" s="9">
         <f>Point!G8</f>
         <v/>
       </c>
       <c r="D17" s="62" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E17" s="62" t="n"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B18" s="9">
         <f>Point!G25</f>
@@ -9101,7 +9107,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B19" s="9">
         <f>Point!G10</f>
@@ -9118,7 +9124,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B20" s="9">
         <f>Point!G13</f>
@@ -9135,7 +9141,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B21" s="9">
         <f>Point!G16</f>
@@ -9163,7 +9169,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B23" s="9">
         <f>Point!G11</f>
@@ -9180,7 +9186,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B24" s="9">
         <f>Point!G26</f>
@@ -9197,7 +9203,7 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B25" s="9">
         <f>Point!G12</f>
@@ -9206,7 +9212,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B26" s="9">
         <f>Point!G9</f>
@@ -9215,7 +9221,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B27" s="9">
         <f>Point!G24</f>
@@ -9224,7 +9230,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B28" s="9">
         <f>Point!G19</f>
@@ -9233,7 +9239,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B29" s="9">
         <f>Point!G14</f>
@@ -9242,7 +9248,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B30" s="9">
         <f>Point!G20</f>
@@ -9251,7 +9257,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="8" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B31" s="9">
         <f>Point!G22</f>
@@ -9260,7 +9266,7 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B32" s="9">
         <f>Point!G21</f>
@@ -9269,7 +9275,7 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B33" s="9">
         <f>Point!G17</f>
@@ -9278,7 +9284,7 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B34" s="9">
         <f>Point!G18</f>
@@ -9287,7 +9293,7 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B35" s="9">
         <f>Point!G27</f>
@@ -9296,7 +9302,7 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B36" s="9">
         <f>Point!G23</f>
@@ -9306,7 +9312,7 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B37" s="9">
         <f>Point!G7</f>
@@ -9315,7 +9321,7 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B38" s="9">
         <f>Point!G15</f>
@@ -9324,7 +9330,7 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="8" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B39" s="9">
         <f>Point!G28</f>
@@ -9336,7 +9342,7 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="10" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B41" s="169">
         <f>Point!G40</f>
@@ -9345,7 +9351,7 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="10" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B42" s="169">
         <f>Point!G41</f>
@@ -9355,7 +9361,7 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="10" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B43" s="169">
         <f>Point!G42</f>
@@ -9365,7 +9371,7 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="10" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B44" s="169">
         <f>Point!G43</f>
@@ -9375,7 +9381,7 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B45" s="169">
         <f>Point!G44</f>
@@ -9385,7 +9391,7 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="10" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B46" s="169">
         <f>Point!G45</f>
@@ -9394,7 +9400,7 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B47" s="169">
         <f>Point!G46</f>
@@ -9403,7 +9409,7 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B48" s="169">
         <f>Point!G47</f>
@@ -9412,7 +9418,7 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="10" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B49" s="169">
         <f>Point!G48</f>
@@ -9421,7 +9427,7 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="10" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B50" s="169">
         <f>Point!G49</f>
@@ -9430,7 +9436,7 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="10" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B51" s="169">
         <f>Point!G50</f>
@@ -9484,7 +9490,7 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="10" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B58" s="9">
         <f>Point!G63</f>

</xml_diff>

<commit_message>
Documents now being requested by _id rather than date
</commit_message>
<xml_diff>
--- a/client/test.xlsx
+++ b/client/test.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="173">
   <si>
     <t>Greenville Convention Center - Alcohol Point Sheets</t>
   </si>
@@ -36,12 +36,15 @@
     <t>Event Number and Name:</t>
   </si>
   <si>
-    <t>TTTTT</t>
+    <t>Day After Halloween</t>
   </si>
   <si>
     <t>Date of Function</t>
   </si>
   <si>
+    <t>10/29/2018</t>
+  </si>
+  <si>
     <t>Bartender(s):</t>
   </si>
   <si>
@@ -222,28 +225,10 @@
     <t>Aristocrat Vodka</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Smirnoff</t>
   </si>
   <si>
-    <t>1.8</t>
-  </si>
-  <si>
-    <t>1.1</t>
-  </si>
-  <si>
     <t>Absolut</t>
-  </si>
-  <si>
-    <t>.5</t>
-  </si>
-  <si>
-    <t>.3</t>
   </si>
   <si>
     <t>Ciroc</t>
@@ -1637,88 +1622,90 @@
         <v>5</v>
       </c>
       <c r="B6" s="21" t="n"/>
-      <c r="C6" s="144" t="s"/>
+      <c r="C6" s="144" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row customHeight="1" ht="15" r="7" spans="1:5">
       <c r="A7" s="21" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="21" t="n"/>
       <c r="C7" s="112" t="s"/>
     </row>
     <row customHeight="1" ht="15" r="8" spans="1:5">
       <c r="A8" s="21" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="21" t="n"/>
       <c r="C8" s="112" t="s"/>
     </row>
     <row customHeight="1" ht="15" r="9" spans="1:5">
       <c r="A9" s="21" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="21" t="n"/>
       <c r="C9" s="112" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="10" spans="1:5">
       <c r="A10" s="21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" s="21" t="n"/>
       <c r="C10" s="51" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D10" s="143" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="11" spans="1:5">
       <c r="A11" s="21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" s="21" t="n"/>
       <c r="C11" s="51" t="n">
         <v>0.21</v>
       </c>
       <c r="D11" s="143" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="12" spans="1:5">
       <c r="A12" s="21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="21" t="n"/>
       <c r="C12" s="145" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="14" spans="1:5">
       <c r="A14" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B14" s="17" t="n"/>
       <c r="C14" s="18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D14" s="146" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E14" s="107" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="15" spans="1:5">
       <c r="A15" s="21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C15" s="147" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D15" s="148">
         <f>ROUND(C15/(1+$C$10),2)</f>
@@ -1727,13 +1714,13 @@
     </row>
     <row customHeight="1" ht="15" r="16" spans="1:5">
       <c r="A16" s="21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C16" s="147" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D16" s="148">
         <f>ROUND(C16/(1+$C$10),2)</f>
@@ -1742,13 +1729,13 @@
     </row>
     <row customHeight="1" ht="15" r="17" spans="1:5">
       <c r="A17" s="21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C17" s="147" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D17" s="148">
         <f>ROUND(C17/(1+$C$10),2)</f>
@@ -1757,13 +1744,13 @@
     </row>
     <row customHeight="1" ht="15" r="18" spans="1:5">
       <c r="A18" s="21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C18" s="147" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D18" s="148">
         <f>ROUND(C18/(1+$C$10),2)</f>
@@ -1772,7 +1759,7 @@
     </row>
     <row hidden="1" r="19" spans="1:5">
       <c r="A19" s="21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B19" s="67" t="n"/>
       <c r="C19" s="23" t="n"/>
@@ -1789,17 +1776,17 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="67" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C21" s="23" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="22" spans="1:5">
       <c r="A22" s="25" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B22" s="25" t="n"/>
       <c r="C22" s="147" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D22" s="148">
         <f>ROUND(C22/(1+$C$10),2)</f>
@@ -1808,11 +1795,11 @@
     </row>
     <row customHeight="1" ht="15" r="23" spans="1:5">
       <c r="A23" s="25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B23" s="25" t="n"/>
       <c r="C23" s="147" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D23" s="148">
         <f>ROUND(C23/(1+$C$10),2)</f>
@@ -1821,11 +1808,11 @@
     </row>
     <row customHeight="1" ht="15" r="24" spans="1:5">
       <c r="A24" s="25" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B24" s="25" t="n"/>
       <c r="C24" s="147" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D24" s="148">
         <f>ROUND(C24/(1+$C$10),2)</f>
@@ -1834,11 +1821,11 @@
     </row>
     <row customHeight="1" ht="15" r="25" spans="1:5">
       <c r="A25" s="25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B25" s="25" t="n"/>
       <c r="C25" s="147" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D25" s="148">
         <f>ROUND(C25/(1+$C$10),2)</f>
@@ -1847,11 +1834,11 @@
     </row>
     <row customHeight="1" ht="15" r="26" spans="1:5">
       <c r="A26" s="25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B26" s="25" t="n"/>
       <c r="C26" s="147" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D26" s="148">
         <f>ROUND(C26/(1+$C$10),2)</f>
@@ -1860,11 +1847,11 @@
     </row>
     <row customHeight="1" ht="15" r="27" spans="1:5">
       <c r="A27" s="25" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B27" s="25" t="n"/>
       <c r="C27" s="147" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D27" s="148">
         <f>ROUND(C27/(1+$C$10),2)</f>
@@ -1876,13 +1863,13 @@
     </row>
     <row customHeight="1" ht="15" r="29" spans="1:5">
       <c r="A29" s="21" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C29" s="147" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D29" s="148">
         <f>ROUND(C29/(1+$C$10),2)</f>
@@ -1891,13 +1878,13 @@
     </row>
     <row customHeight="1" ht="15" r="30" spans="1:5">
       <c r="A30" s="21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C30" s="147" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D30" s="148">
         <f>ROUND(C30/(1+$C$10),2)</f>
@@ -1973,7 +1960,7 @@
   <sheetData>
     <row customHeight="1" ht="15.75" r="1" spans="1:40">
       <c r="A1" s="117" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="2" spans="1:40">
@@ -1982,10 +1969,10 @@
         <v/>
       </c>
       <c r="Q2" s="134" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AK2" s="134" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="3" spans="1:40">
@@ -1994,45 +1981,45 @@
         <v/>
       </c>
       <c r="Q3" s="136" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="V3" s="135" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AA3" s="135" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AF3" s="135" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:40">
       <c r="A4" s="130" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C4" s="29">
         <f>IF(Input!C9="Y","Host","Cash")</f>
         <v/>
       </c>
       <c r="E4" s="128" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H4" s="97" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I4" s="97" t="n"/>
       <c r="J4" s="98" t="n"/>
       <c r="K4" s="97" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L4" s="97" t="s">
+        <v>54</v>
+      </c>
+      <c r="M4" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="M4" s="97" t="s">
-        <v>52</v>
-      </c>
       <c r="N4" s="128" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="Q4" s="53" t="n"/>
       <c r="R4" s="53" t="n"/>
@@ -2053,122 +2040,122 @@
     </row>
     <row r="5" spans="1:40">
       <c r="A5" s="130" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="133">
         <f>Input!C8</f>
         <v/>
       </c>
       <c r="E5" s="128" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F5" s="128" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G5" s="128" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H5" s="100" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I5" s="100" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J5" s="98" t="n"/>
       <c r="K5" s="100" t="s">
+        <v>60</v>
+      </c>
+      <c r="L5" s="100" t="s">
+        <v>60</v>
+      </c>
+      <c r="M5" s="100" t="s">
+        <v>61</v>
+      </c>
+      <c r="N5" s="128" t="s">
+        <v>62</v>
+      </c>
+      <c r="O5" s="128" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q5" s="135" t="s">
+        <v>55</v>
+      </c>
+      <c r="R5" s="135" t="s">
+        <v>56</v>
+      </c>
+      <c r="S5" s="135" t="s">
+        <v>57</v>
+      </c>
+      <c r="T5" s="135" t="s">
         <v>59</v>
       </c>
-      <c r="L5" s="100" t="s">
+      <c r="V5" s="135" t="s">
+        <v>55</v>
+      </c>
+      <c r="W5" s="135" t="s">
+        <v>56</v>
+      </c>
+      <c r="X5" s="135" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y5" s="135" t="s">
         <v>59</v>
       </c>
-      <c r="M5" s="100" t="s">
-        <v>60</v>
-      </c>
-      <c r="N5" s="128" t="s">
-        <v>61</v>
-      </c>
-      <c r="O5" s="128" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q5" s="135" t="s">
-        <v>54</v>
-      </c>
-      <c r="R5" s="135" t="s">
+      <c r="AA5" s="135" t="s">
         <v>55</v>
       </c>
-      <c r="S5" s="135" t="s">
+      <c r="AB5" s="135" t="s">
         <v>56</v>
       </c>
-      <c r="T5" s="135" t="s">
-        <v>58</v>
-      </c>
-      <c r="V5" s="135" t="s">
-        <v>54</v>
-      </c>
-      <c r="W5" s="135" t="s">
+      <c r="AC5" s="135" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD5" s="135" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF5" s="135" t="s">
         <v>55</v>
       </c>
-      <c r="X5" s="135" t="s">
+      <c r="AG5" s="135" t="s">
         <v>56</v>
       </c>
-      <c r="Y5" s="135" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA5" s="135" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB5" s="135" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC5" s="135" t="s">
-        <v>56</v>
-      </c>
-      <c r="AD5" s="135" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF5" s="135" t="s">
-        <v>54</v>
-      </c>
-      <c r="AG5" s="135" t="s">
-        <v>55</v>
-      </c>
       <c r="AH5" s="135" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AI5" s="135" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AK5" s="104" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AL5" s="134" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AM5" s="134" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AN5" s="101" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row customHeight="1" ht="14.1" r="6" spans="1:40">
       <c r="A6" s="129" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B6" s="132" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="47" t="s">
-        <v>66</v>
-      </c>
-      <c r="F6" s="47" t="s">
-        <v>67</v>
+        <v>32</v>
+      </c>
+      <c r="E6" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G6" s="32">
         <f>E6-F6</f>
@@ -2285,16 +2272,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="7" spans="1:40">
       <c r="C7" s="31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="47" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" s="47" t="s">
-        <v>70</v>
+        <v>23</v>
+      </c>
+      <c r="E7" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G7" s="32">
         <f>E7-F7</f>
@@ -2411,16 +2398,16 @@
     </row>
     <row customHeight="1" ht="14.1" r="8" spans="1:40">
       <c r="C8" s="31" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" s="47" t="s">
-        <v>73</v>
+        <v>26</v>
+      </c>
+      <c r="E8" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="47" t="n">
+        <v>0</v>
       </c>
       <c r="G8" s="32">
         <f>E8-F8</f>
@@ -2537,10 +2524,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="9" spans="1:40">
       <c r="C9" s="31" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E9" s="47" t="n">
         <v>0</v>
@@ -2663,13 +2650,13 @@
     </row>
     <row customHeight="1" ht="14.1" r="10" spans="1:40">
       <c r="B10" s="121" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E10" s="47" t="n">
         <v>0</v>
@@ -2792,10 +2779,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="11" spans="1:40">
       <c r="C11" s="31" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E11" s="47" t="n">
         <v>0</v>
@@ -2918,10 +2905,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="12" spans="1:40">
       <c r="C12" s="31" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E12" s="47" t="n">
         <v>0</v>
@@ -3044,13 +3031,13 @@
     </row>
     <row customHeight="1" ht="14.1" r="13" spans="1:40">
       <c r="B13" s="132" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E13" s="47" t="n">
         <v>0</v>
@@ -3173,10 +3160,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="14" spans="1:40">
       <c r="C14" s="31" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E14" s="47" t="n">
         <v>0</v>
@@ -3299,10 +3286,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="15" spans="1:40">
       <c r="C15" s="31" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E15" s="47" t="n">
         <v>0</v>
@@ -3425,13 +3412,13 @@
     </row>
     <row customHeight="1" ht="14.1" r="16" spans="1:40">
       <c r="B16" s="121" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E16" s="47" t="n">
         <v>0</v>
@@ -3554,10 +3541,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="17" spans="1:40">
       <c r="C17" s="31" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E17" s="47" t="n">
         <v>0</v>
@@ -3680,10 +3667,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="18" spans="1:40">
       <c r="C18" s="31" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E18" s="47" t="n">
         <v>0</v>
@@ -3806,13 +3793,13 @@
     </row>
     <row customHeight="1" ht="14.1" r="19" spans="1:40">
       <c r="B19" s="121" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E19" s="47" t="n">
         <v>0</v>
@@ -3935,10 +3922,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="20" spans="1:40">
       <c r="C20" s="31" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E20" s="47" t="n">
         <v>0</v>
@@ -4061,13 +4048,13 @@
     </row>
     <row customHeight="1" ht="14.1" r="21" spans="1:40">
       <c r="B21" s="132" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E21" s="47" t="n">
         <v>0</v>
@@ -4190,10 +4177,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="22" spans="1:40">
       <c r="C22" s="31" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E22" s="47" t="n">
         <v>0</v>
@@ -4316,13 +4303,13 @@
     </row>
     <row customHeight="1" ht="14.1" r="23" spans="1:40">
       <c r="B23" s="132" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E23" s="47" t="n">
         <v>0</v>
@@ -4445,10 +4432,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="24" spans="1:40">
       <c r="C24" s="31" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E24" s="47" t="n">
         <v>0</v>
@@ -4571,13 +4558,13 @@
     </row>
     <row customHeight="1" ht="14.1" r="25" spans="1:40">
       <c r="B25" s="121" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E25" s="47" t="n">
         <v>0</v>
@@ -4700,10 +4687,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="26" spans="1:40">
       <c r="C26" s="31" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E26" s="47" t="n">
         <v>0</v>
@@ -4826,10 +4813,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="27" spans="1:40">
       <c r="C27" s="31" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E27" s="47" t="n">
         <v>0</v>
@@ -4952,10 +4939,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="28" spans="1:40">
       <c r="C28" s="31" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D28" s="31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E28" s="47" t="n">
         <v>0</v>
@@ -5078,13 +5065,13 @@
     </row>
     <row customHeight="1" ht="14.1" r="29" spans="1:40">
       <c r="B29" s="123" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C29" s="105" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E29" s="47" t="n">
         <v>0</v>
@@ -5207,10 +5194,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="30" spans="1:40">
       <c r="C30" s="48" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E30" s="47" t="n">
         <v>0</v>
@@ -5333,10 +5320,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="31" spans="1:40">
       <c r="C31" s="105" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E31" s="47" t="n">
         <v>0</v>
@@ -5459,10 +5446,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="32" spans="1:40">
       <c r="C32" s="105" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E32" s="47" t="n">
         <v>0</v>
@@ -5604,10 +5591,10 @@
       <c r="A34" s="35" t="n"/>
       <c r="B34" s="35" t="n"/>
       <c r="C34" s="44" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D34" s="44" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E34" s="32">
         <f>Q34</f>
@@ -5682,7 +5669,7 @@
       <c r="B35" s="35" t="n"/>
       <c r="C35" s="35" t="n"/>
       <c r="D35" s="44" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E35" s="32">
         <f>V35</f>
@@ -5741,7 +5728,7 @@
       <c r="B36" s="35" t="n"/>
       <c r="C36" s="35" t="n"/>
       <c r="D36" s="44" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E36" s="32">
         <f>AA36</f>
@@ -5804,7 +5791,7 @@
       <c r="B37" s="35" t="n"/>
       <c r="C37" s="35" t="n"/>
       <c r="D37" s="44" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E37" s="32">
         <f>AF37</f>
@@ -5867,7 +5854,7 @@
       <c r="B38" s="35" t="n"/>
       <c r="C38" s="35" t="n"/>
       <c r="D38" s="44" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E38" s="32">
         <f>SUM(E34:E37)</f>
@@ -5922,27 +5909,27 @@
       <c r="N39" s="35" t="n"/>
       <c r="O39" s="35" t="n"/>
       <c r="Q39" s="134" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="V39" s="134" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AK39" s="134" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AL39" s="134" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row customHeight="1" ht="14.1" r="40" spans="1:40">
       <c r="A40" s="129" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B40" s="116" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E40" s="50" t="n">
         <v>0</v>
@@ -6024,10 +6011,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="41" spans="1:40">
       <c r="B41" s="119" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D41" s="31" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E41" s="50" t="n">
         <v>0</v>
@@ -6110,10 +6097,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="42" spans="1:40">
       <c r="B42" s="119" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D42" s="31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E42" s="50" t="n">
         <v>0</v>
@@ -6196,10 +6183,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="43" spans="1:40">
       <c r="B43" s="119" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D43" s="31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E43" s="50" t="n">
         <v>0</v>
@@ -6282,10 +6269,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="44" spans="1:40">
       <c r="B44" s="119" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D44" s="31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E44" s="50" t="n">
         <v>0</v>
@@ -6368,10 +6355,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="45" spans="1:40">
       <c r="B45" s="119" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D45" s="31" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E45" s="50" t="n">
         <v>0</v>
@@ -6454,10 +6441,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="46" spans="1:40">
       <c r="B46" s="119" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D46" s="31" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E46" s="50" t="n">
         <v>0</v>
@@ -6540,10 +6527,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="47" spans="1:40">
       <c r="B47" s="119" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D47" s="31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E47" s="50" t="n">
         <v>0</v>
@@ -6626,10 +6613,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="48" spans="1:40">
       <c r="B48" s="119" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D48" s="31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E48" s="50" t="n">
         <v>0</v>
@@ -6712,10 +6699,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="49" spans="1:40">
       <c r="B49" s="119" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D49" s="31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E49" s="50" t="n">
         <v>0</v>
@@ -6798,10 +6785,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="50" spans="1:40">
       <c r="B50" s="119" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D50" s="31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E50" s="50" t="n">
         <v>0</v>
@@ -6885,7 +6872,7 @@
     <row customHeight="1" ht="14.1" r="51" spans="1:40">
       <c r="B51" s="126" t="n"/>
       <c r="D51" s="31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E51" s="50" t="n"/>
       <c r="F51" s="50" t="n"/>
@@ -6965,7 +6952,7 @@
     <row customHeight="1" ht="14.1" r="52" spans="1:40">
       <c r="B52" s="126" t="n"/>
       <c r="D52" s="31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E52" s="50" t="n"/>
       <c r="F52" s="50" t="n"/>
@@ -7063,10 +7050,10 @@
       <c r="A54" s="35" t="n"/>
       <c r="B54" s="35" t="n"/>
       <c r="C54" s="43" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D54" s="44" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E54" s="41">
         <f>Q54</f>
@@ -7133,7 +7120,7 @@
       <c r="B55" s="35" t="n"/>
       <c r="C55" s="35" t="n"/>
       <c r="D55" s="44" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E55" s="41">
         <f>V55</f>
@@ -7192,7 +7179,7 @@
       <c r="B56" s="35" t="n"/>
       <c r="C56" s="35" t="n"/>
       <c r="D56" s="44" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E56" s="41">
         <f>SUM(E54:E55)</f>
@@ -7247,18 +7234,18 @@
       <c r="N57" s="35" t="n"/>
       <c r="O57" s="35" t="n"/>
       <c r="AK57" s="134" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row customHeight="1" ht="14.1" r="58" spans="1:40">
       <c r="A58" s="129" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B58" s="116" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D58" s="44" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E58" s="47" t="n">
         <v>0</v>
@@ -7321,10 +7308,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="59" spans="1:40">
       <c r="B59" s="116" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D59" s="44" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E59" s="47" t="n">
         <v>0</v>
@@ -7387,10 +7374,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="60" spans="1:40">
       <c r="B60" s="116" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D60" s="44" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E60" s="47" t="n">
         <v>0</v>
@@ -7453,13 +7440,17 @@
     </row>
     <row customHeight="1" ht="14.1" r="61" spans="1:40">
       <c r="B61" s="116" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D61" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="E61" s="106" t="n"/>
-      <c r="F61" s="47" t="n"/>
+        <v>115</v>
+      </c>
+      <c r="E61" s="106" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" s="47" t="n">
+        <v>0</v>
+      </c>
       <c r="G61" s="32">
         <f>E61-F61</f>
         <v/>
@@ -7515,10 +7506,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="62" spans="1:40">
       <c r="B62" s="116" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D62" s="44" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E62" s="47" t="n">
         <v>0</v>
@@ -7580,10 +7571,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="63" spans="1:40">
       <c r="B63" s="116" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D63" s="44" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E63" s="47" t="n">
         <v>0</v>
@@ -7665,10 +7656,10 @@
       <c r="A65" s="35" t="n"/>
       <c r="B65" s="35" t="n"/>
       <c r="C65" s="43" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D65" s="44" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E65" s="32">
         <f>Q65</f>
@@ -7731,7 +7722,7 @@
       <c r="B66" s="35" t="n"/>
       <c r="C66" s="35" t="n"/>
       <c r="D66" s="44" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E66" s="32">
         <f>SUM(E65:E65)</f>
@@ -7782,7 +7773,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="68" spans="1:40">
       <c r="A68" s="45" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B68" s="46" t="n"/>
       <c r="C68" s="116">
@@ -7798,28 +7789,28 @@
     </row>
     <row customFormat="1" hidden="1" r="70" s="52" spans="1:40">
       <c r="B70" s="52" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C70" s="52" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row customFormat="1" hidden="1" r="71" s="52" spans="1:40">
       <c r="B71" s="52" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C71" s="52" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row customFormat="1" hidden="1" r="72" s="52" spans="1:40">
       <c r="B72" s="52" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row customFormat="1" hidden="1" r="73" s="52" spans="1:40">
       <c r="B73" s="103" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -7927,7 +7918,7 @@
   <sheetData>
     <row customHeight="1" ht="15.75" r="1" spans="1:15">
       <c r="A1" s="137" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E1" s="65" t="n"/>
       <c r="F1" s="68" t="n"/>
@@ -7956,18 +7947,18 @@
     <row customHeight="1" ht="6.95" r="4" spans="1:15"/>
     <row r="5" spans="1:15">
       <c r="B5" s="18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="21" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B6" s="18">
         <f>ROUND(Point!G34*Point!L34,0)</f>
@@ -7984,7 +7975,7 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="21" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B7" s="18">
         <f>ROUND(Point!G35*Point!L35,0)</f>
@@ -8001,7 +7992,7 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="21" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B8" s="18">
         <f>ROUND(Point!G36*Point!L36,0)</f>
@@ -8018,7 +8009,7 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="21" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B9" s="18">
         <f>ROUND(Point!G37*Point!L37,0)</f>
@@ -8035,7 +8026,7 @@
     </row>
     <row customFormat="1" r="10" s="74" spans="1:15">
       <c r="A10" s="70" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B10" s="71">
         <f>SUM(B6:B9)</f>
@@ -8059,7 +8050,7 @@
     <row customHeight="1" ht="6.95" r="11" spans="1:15"/>
     <row r="12" spans="1:15">
       <c r="A12" s="21" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B12" s="18">
         <f>ROUND(Point!G54*Point!L54,0)</f>
@@ -8076,7 +8067,7 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B13" s="18">
         <f>ROUND(Point!G55*Point!L55,0)</f>
@@ -8093,7 +8084,7 @@
     </row>
     <row customFormat="1" r="14" s="74" spans="1:15">
       <c r="A14" s="70" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B14" s="71">
         <f>SUM(B12:B13)</f>
@@ -8117,7 +8108,7 @@
     <row customHeight="1" ht="6.95" r="15" spans="1:15"/>
     <row r="16" spans="1:15">
       <c r="A16" s="21" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B16" s="18">
         <f>ROUND(Point!G58*Point!L58,0)</f>
@@ -8134,7 +8125,7 @@
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="21" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B17" s="18">
         <f>ROUND(Point!G59*Point!L59,0)</f>
@@ -8151,7 +8142,7 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="21" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B18" s="18">
         <f>ROUND(Point!G60*Point!L60,0)</f>
@@ -8168,7 +8159,7 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="21" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B19" s="18">
         <f>ROUND(Point!G61*Point!L61,0)</f>
@@ -8185,7 +8176,7 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" s="21" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B20" s="18">
         <f>ROUND(Point!G62*Point!L62,0)</f>
@@ -8202,7 +8193,7 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="21" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B21" s="18">
         <f>ROUND(Point!G63*Point!L63,0)</f>
@@ -8219,7 +8210,7 @@
     </row>
     <row customFormat="1" r="22" s="74" spans="1:15">
       <c r="A22" s="70" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B22" s="71">
         <f>SUM(B16:B21)</f>
@@ -8243,11 +8234,11 @@
     <row customHeight="1" ht="6.95" r="23" spans="1:15"/>
     <row r="24" spans="1:15">
       <c r="A24" s="75" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B24" s="76" t="n"/>
       <c r="C24" s="77" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D24" s="160">
         <f>ROUND(SUM(D10,D14,D22),2)</f>
@@ -8264,7 +8255,7 @@
         <v/>
       </c>
       <c r="C25" s="77" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D25" s="159">
         <f>IF(Input!C9="Y",ROUND(Summary!D24*B25,2),0)</f>
@@ -8273,14 +8264,14 @@
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="75" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B26" s="80">
         <f>Input!C10</f>
         <v/>
       </c>
       <c r="C26" s="77" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D26" s="159">
         <f>ROUND(SUM(D24:D25)*B26,2)</f>
@@ -8294,7 +8285,7 @@
       </c>
       <c r="B27" s="76" t="n"/>
       <c r="C27" s="77" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D27" s="159">
         <f>SUM(D24:D26)</f>
@@ -8303,11 +8294,11 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="75" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B28" s="76" t="n"/>
       <c r="C28" s="77" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D28" s="159">
         <f>Input!C12</f>
@@ -8321,7 +8312,7 @@
       </c>
       <c r="B29" s="76" t="n"/>
       <c r="C29" s="77" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D29" s="159">
         <f>IF(Input!C9="Y",Summary!D27,0)</f>
@@ -8331,7 +8322,7 @@
     <row r="30" spans="1:15">
       <c r="B30" s="76" t="n"/>
       <c r="C30" s="77" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D30" s="159">
         <f>D29+D28-D27</f>
@@ -8347,25 +8338,25 @@
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="140" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row customHeight="1" ht="6.95" r="34" spans="1:15"/>
     <row r="35" spans="1:15">
       <c r="A35" s="140" t="n"/>
       <c r="B35" s="83" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C35" s="71" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D35" s="71" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="36" spans="1:15">
       <c r="A36" s="21" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B36" s="158">
         <f>D6</f>
@@ -8382,7 +8373,7 @@
     </row>
     <row r="37" spans="1:15">
       <c r="A37" s="21" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B37" s="158">
         <f>D7</f>
@@ -8399,7 +8390,7 @@
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="21" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B38" s="158">
         <f>D8</f>
@@ -8416,7 +8407,7 @@
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="21" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B39" s="158">
         <f>D9</f>
@@ -8433,7 +8424,7 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="70" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B40" s="160">
         <f>SUM(B36:B39)</f>
@@ -8451,7 +8442,7 @@
     <row customHeight="1" ht="6.95" r="41" spans="1:15"/>
     <row r="42" spans="1:15">
       <c r="A42" s="70" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B42" s="86">
         <f>Input!D19</f>
@@ -8463,7 +8454,7 @@
     <row customHeight="1" ht="6.95" r="43" spans="1:15"/>
     <row r="44" spans="1:15">
       <c r="A44" s="21" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B44" s="158">
         <f>D12</f>
@@ -8480,7 +8471,7 @@
     </row>
     <row r="45" spans="1:15">
       <c r="A45" s="21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B45" s="158">
         <f>D13</f>
@@ -8497,7 +8488,7 @@
     </row>
     <row r="46" spans="1:15">
       <c r="A46" s="70" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B46" s="160">
         <f>SUM(B44:B45)</f>
@@ -8515,7 +8506,7 @@
     <row customHeight="1" ht="6.95" r="47" spans="1:15"/>
     <row r="48" spans="1:15">
       <c r="A48" s="21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B48" s="158">
         <f>D22</f>
@@ -8532,7 +8523,7 @@
     </row>
     <row r="49" spans="1:15">
       <c r="A49" s="70" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B49" s="160">
         <f>SUM(B48:B48)</f>
@@ -8550,7 +8541,7 @@
     <row customHeight="1" ht="6.95" r="50" spans="1:15"/>
     <row r="51" spans="1:15">
       <c r="A51" s="89" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B51" s="160">
         <f>B40+B46+B49</f>
@@ -8567,7 +8558,7 @@
     </row>
     <row customFormat="1" hidden="1" r="55" s="68" spans="1:15">
       <c r="F55" s="90" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G55" s="162">
         <f>Input!C12</f>
@@ -8576,7 +8567,7 @@
     </row>
     <row customFormat="1" hidden="1" r="56" s="68" spans="1:15">
       <c r="F56" s="90" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="G56" s="162">
         <f>ROUND(IF(Input!C10=0,0,G55-(G55/(1+Input!C10))),2)</f>
@@ -8585,7 +8576,7 @@
     </row>
     <row customFormat="1" hidden="1" r="57" s="68" spans="1:15">
       <c r="F57" s="90" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="G57" s="162">
         <f>D14</f>
@@ -8594,7 +8585,7 @@
     </row>
     <row customFormat="1" hidden="1" r="58" s="68" spans="1:15">
       <c r="F58" s="90" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G58" s="162">
         <f>D22</f>
@@ -8603,7 +8594,7 @@
     </row>
     <row customFormat="1" hidden="1" r="59" s="68" spans="1:15">
       <c r="F59" s="90" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G59" s="162">
         <f>G55-SUM(G56:G58)</f>
@@ -8612,7 +8603,7 @@
     </row>
     <row customFormat="1" hidden="1" r="60" s="68" spans="1:15">
       <c r="F60" s="90" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G60" s="162">
         <f>G55-SUM(G56:G59)</f>
@@ -8624,7 +8615,7 @@
     </row>
     <row customFormat="1" hidden="1" r="62" s="68" spans="1:15">
       <c r="F62" s="90" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G62" s="162">
         <f>G59</f>
@@ -8633,7 +8624,7 @@
     </row>
     <row customFormat="1" hidden="1" r="63" s="68" spans="1:15">
       <c r="F63" s="90" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="G63" s="93">
         <f>Point!G38</f>
@@ -8642,7 +8633,7 @@
     </row>
     <row customFormat="1" hidden="1" r="64" s="68" spans="1:15">
       <c r="F64" s="90" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G64" s="93">
         <f>26.40825/G62*G63</f>
@@ -8652,24 +8643,24 @@
     <row customFormat="1" hidden="1" r="65" s="68" spans="1:15"/>
     <row customFormat="1" hidden="1" r="66" s="68" spans="1:15">
       <c r="G66" s="94" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H66" s="94" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I66" s="94" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K66" s="94" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="N66" s="94" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row customFormat="1" hidden="1" r="67" s="68" spans="1:15">
       <c r="F67" s="90" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G67" s="93">
         <f>Point!G34</f>
@@ -8706,7 +8697,7 @@
     </row>
     <row customFormat="1" hidden="1" r="68" s="68" spans="1:15">
       <c r="F68" s="90" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G68" s="93">
         <f>Point!G35</f>
@@ -8743,7 +8734,7 @@
     </row>
     <row customFormat="1" hidden="1" r="69" s="68" spans="1:15">
       <c r="F69" s="90" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="G69" s="93">
         <f>Point!G36</f>
@@ -8780,7 +8771,7 @@
     </row>
     <row customFormat="1" hidden="1" r="70" s="68" spans="1:15">
       <c r="F70" s="90" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="G70" s="93">
         <f>Point!G37</f>
@@ -8895,14 +8886,14 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B1" s="2">
         <f>Input!C5</f>
         <v/>
       </c>
       <c r="D1" s="141" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -8915,7 +8906,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B3" s="2">
         <f>Summary!A25</f>
@@ -8928,7 +8919,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B4" s="2">
         <f>Input!C6</f>
@@ -8943,22 +8934,22 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B6" s="166">
         <f>Summary!D10</f>
         <v/>
       </c>
       <c r="F6" s="167" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="G6" s="167" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B7" s="166">
         <f>Summary!D14</f>
@@ -8968,7 +8959,7 @@
         <v>454598</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F7" s="168">
         <f>G13</f>
@@ -8978,7 +8969,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B8" s="166">
         <f>Summary!D22</f>
@@ -8988,7 +8979,7 @@
         <v>464691</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F8" s="168" t="n"/>
       <c r="G8" s="168">
@@ -9003,7 +8994,7 @@
         <v>464692</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F9" s="168" t="n"/>
       <c r="G9" s="168">
@@ -9016,7 +9007,7 @@
         <v>464693</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F10" s="168" t="n"/>
       <c r="G10" s="168">
@@ -9026,7 +9017,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="5" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B11" s="166">
         <f>Summary!C40</f>
@@ -9036,7 +9027,7 @@
         <v>454598</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="F11" s="168" t="n"/>
       <c r="G11" s="168">
@@ -9046,7 +9037,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="5" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B12" s="166">
         <f>+Summary!C46</f>
@@ -9056,7 +9047,7 @@
         <v>202220</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F12" s="168" t="n"/>
       <c r="G12" s="168">
@@ -9066,7 +9057,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="5" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B13" s="166">
         <f>+Summary!C49</f>
@@ -9089,20 +9080,20 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B17" s="9">
         <f>Point!G8</f>
         <v/>
       </c>
       <c r="D17" s="62" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E17" s="62" t="n"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="8" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B18" s="9">
         <f>Point!G25</f>
@@ -9119,7 +9110,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="8" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B19" s="9">
         <f>Point!G10</f>
@@ -9136,7 +9127,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="8" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B20" s="9">
         <f>Point!G13</f>
@@ -9153,7 +9144,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="8" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B21" s="9">
         <f>Point!G16</f>
@@ -9170,7 +9161,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B22" s="9">
         <f>Point!G6</f>
@@ -9181,7 +9172,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="8" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B23" s="9">
         <f>Point!G11</f>
@@ -9198,7 +9189,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B24" s="9">
         <f>Point!G26</f>
@@ -9215,7 +9206,7 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="8" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B25" s="9">
         <f>Point!G12</f>
@@ -9224,7 +9215,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="8" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B26" s="9">
         <f>Point!G9</f>
@@ -9233,7 +9224,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="8" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B27" s="9">
         <f>Point!G24</f>
@@ -9242,7 +9233,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="8" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B28" s="9">
         <f>Point!G19</f>
@@ -9251,7 +9242,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="8" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B29" s="9">
         <f>Point!G14</f>
@@ -9260,7 +9251,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="8" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B30" s="9">
         <f>Point!G20</f>
@@ -9269,7 +9260,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="8" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B31" s="9">
         <f>Point!G22</f>
@@ -9278,7 +9269,7 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B32" s="9">
         <f>Point!G21</f>
@@ -9287,7 +9278,7 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B33" s="9">
         <f>Point!G17</f>
@@ -9296,7 +9287,7 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B34" s="9">
         <f>Point!G18</f>
@@ -9305,7 +9296,7 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="8" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B35" s="9">
         <f>Point!G27</f>
@@ -9314,7 +9305,7 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="8" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B36" s="9">
         <f>Point!G23</f>
@@ -9324,7 +9315,7 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B37" s="9">
         <f>Point!G7</f>
@@ -9333,7 +9324,7 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="8" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B38" s="9">
         <f>Point!G15</f>
@@ -9342,7 +9333,7 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="8" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B39" s="9">
         <f>Point!G28</f>
@@ -9354,7 +9345,7 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="10" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B41" s="169">
         <f>Point!G40</f>
@@ -9363,7 +9354,7 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="10" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B42" s="169">
         <f>Point!G41</f>
@@ -9373,7 +9364,7 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="10" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B43" s="169">
         <f>Point!G42</f>
@@ -9383,7 +9374,7 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="10" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B44" s="169">
         <f>Point!G43</f>
@@ -9393,7 +9384,7 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="10" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B45" s="169">
         <f>Point!G44</f>
@@ -9403,7 +9394,7 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="10" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B46" s="169">
         <f>Point!G45</f>
@@ -9412,7 +9403,7 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="10" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B47" s="169">
         <f>Point!G46</f>
@@ -9421,7 +9412,7 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="10" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B48" s="169">
         <f>Point!G47</f>
@@ -9430,7 +9421,7 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="10" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B49" s="169">
         <f>Point!G48</f>
@@ -9439,7 +9430,7 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="10" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B50" s="169">
         <f>Point!G49</f>
@@ -9448,7 +9439,7 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="10" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B51" s="169">
         <f>Point!G50</f>
@@ -9457,7 +9448,7 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B53" s="9">
         <f>Point!G58</f>
@@ -9466,7 +9457,7 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B54" s="9">
         <f>Point!G59</f>
@@ -9475,7 +9466,7 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B55" s="9">
         <f>Point!G60</f>
@@ -9484,7 +9475,7 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B56" s="9">
         <f>Point!G61</f>
@@ -9493,7 +9484,7 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B57" s="9">
         <f>Point!G62</f>
@@ -9502,7 +9493,7 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="10" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B58" s="9">
         <f>Point!G63</f>

</xml_diff>

<commit_message>
allows user to specify recipient's email. validation not implemented'
</commit_message>
<xml_diff>
--- a/client/test.xlsx
+++ b/client/test.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="174">
   <si>
     <t>Greenville Convention Center - Alcohol Point Sheets</t>
   </si>
@@ -36,15 +36,12 @@
     <t>Event Number and Name:</t>
   </si>
   <si>
-    <t>Day After Halloween</t>
+    <t>Fiddlesticks</t>
   </si>
   <si>
     <t>Date of Function</t>
   </si>
   <si>
-    <t>10/29/2018</t>
-  </si>
-  <si>
     <t>Bartender(s):</t>
   </si>
   <si>
@@ -223,6 +220,12 @@
   </si>
   <si>
     <t>Aristocrat Vodka</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
   <si>
     <t>Smirnoff</t>
@@ -1622,90 +1625,88 @@
         <v>5</v>
       </c>
       <c r="B6" s="21" t="n"/>
-      <c r="C6" s="144" t="s">
-        <v>6</v>
-      </c>
+      <c r="C6" s="144" t="s"/>
     </row>
     <row customHeight="1" ht="15" r="7" spans="1:5">
       <c r="A7" s="21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="21" t="n"/>
       <c r="C7" s="112" t="s"/>
     </row>
     <row customHeight="1" ht="15" r="8" spans="1:5">
       <c r="A8" s="21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="21" t="n"/>
       <c r="C8" s="112" t="s"/>
     </row>
     <row customHeight="1" ht="15" r="9" spans="1:5">
       <c r="A9" s="21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="21" t="n"/>
       <c r="C9" s="112" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="10" spans="1:5">
       <c r="A10" s="21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="21" t="n"/>
       <c r="C10" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="143" t="s">
         <v>12</v>
-      </c>
-      <c r="D10" s="143" t="s">
-        <v>13</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="11" spans="1:5">
       <c r="A11" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="21" t="n"/>
       <c r="C11" s="51" t="n">
         <v>0.21</v>
       </c>
       <c r="D11" s="143" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="12" spans="1:5">
       <c r="A12" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="21" t="n"/>
       <c r="C12" s="145" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="14" spans="1:5">
       <c r="A14" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="17" t="n"/>
       <c r="C14" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="146" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="146" t="s">
+      <c r="E14" s="107" t="s">
         <v>20</v>
-      </c>
-      <c r="E14" s="107" t="s">
-        <v>21</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="15" spans="1:5">
       <c r="A15" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="C15" s="147" t="s">
         <v>23</v>
-      </c>
-      <c r="C15" s="147" t="s">
-        <v>24</v>
       </c>
       <c r="D15" s="148">
         <f>ROUND(C15/(1+$C$10),2)</f>
@@ -1714,13 +1715,13 @@
     </row>
     <row customHeight="1" ht="15" r="16" spans="1:5">
       <c r="A16" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="C16" s="147" t="s">
         <v>26</v>
-      </c>
-      <c r="C16" s="147" t="s">
-        <v>27</v>
       </c>
       <c r="D16" s="148">
         <f>ROUND(C16/(1+$C$10),2)</f>
@@ -1729,13 +1730,13 @@
     </row>
     <row customHeight="1" ht="15" r="17" spans="1:5">
       <c r="A17" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="C17" s="147" t="s">
         <v>29</v>
-      </c>
-      <c r="C17" s="147" t="s">
-        <v>30</v>
       </c>
       <c r="D17" s="148">
         <f>ROUND(C17/(1+$C$10),2)</f>
@@ -1744,13 +1745,13 @@
     </row>
     <row customHeight="1" ht="15" r="18" spans="1:5">
       <c r="A18" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="C18" s="147" t="s">
         <v>32</v>
-      </c>
-      <c r="C18" s="147" t="s">
-        <v>33</v>
       </c>
       <c r="D18" s="148">
         <f>ROUND(C18/(1+$C$10),2)</f>
@@ -1759,7 +1760,7 @@
     </row>
     <row hidden="1" r="19" spans="1:5">
       <c r="A19" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="67" t="n"/>
       <c r="C19" s="23" t="n"/>
@@ -1776,17 +1777,17 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="67" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="23" t="n"/>
     </row>
     <row customHeight="1" ht="15" r="22" spans="1:5">
       <c r="A22" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" s="25" t="n"/>
       <c r="C22" s="147" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D22" s="148">
         <f>ROUND(C22/(1+$C$10),2)</f>
@@ -1795,11 +1796,11 @@
     </row>
     <row customHeight="1" ht="15" r="23" spans="1:5">
       <c r="A23" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="25" t="n"/>
       <c r="C23" s="147" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D23" s="148">
         <f>ROUND(C23/(1+$C$10),2)</f>
@@ -1808,11 +1809,11 @@
     </row>
     <row customHeight="1" ht="15" r="24" spans="1:5">
       <c r="A24" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" s="25" t="n"/>
       <c r="C24" s="147" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D24" s="148">
         <f>ROUND(C24/(1+$C$10),2)</f>
@@ -1821,11 +1822,11 @@
     </row>
     <row customHeight="1" ht="15" r="25" spans="1:5">
       <c r="A25" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="25" t="n"/>
       <c r="C25" s="147" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D25" s="148">
         <f>ROUND(C25/(1+$C$10),2)</f>
@@ -1834,11 +1835,11 @@
     </row>
     <row customHeight="1" ht="15" r="26" spans="1:5">
       <c r="A26" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="25" t="n"/>
       <c r="C26" s="147" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D26" s="148">
         <f>ROUND(C26/(1+$C$10),2)</f>
@@ -1847,11 +1848,11 @@
     </row>
     <row customHeight="1" ht="15" r="27" spans="1:5">
       <c r="A27" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" s="25" t="n"/>
       <c r="C27" s="147" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D27" s="148">
         <f>ROUND(C27/(1+$C$10),2)</f>
@@ -1863,13 +1864,13 @@
     </row>
     <row customHeight="1" ht="15" r="29" spans="1:5">
       <c r="A29" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="C29" s="147" t="s">
         <v>43</v>
-      </c>
-      <c r="C29" s="147" t="s">
-        <v>44</v>
       </c>
       <c r="D29" s="148">
         <f>ROUND(C29/(1+$C$10),2)</f>
@@ -1878,13 +1879,13 @@
     </row>
     <row customHeight="1" ht="15" r="30" spans="1:5">
       <c r="A30" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="21" t="s">
-        <v>46</v>
-      </c>
       <c r="C30" s="147" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D30" s="148">
         <f>ROUND(C30/(1+$C$10),2)</f>
@@ -1960,7 +1961,7 @@
   <sheetData>
     <row customHeight="1" ht="15.75" r="1" spans="1:40">
       <c r="A1" s="117" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="2" spans="1:40">
@@ -1969,10 +1970,10 @@
         <v/>
       </c>
       <c r="Q2" s="134" t="s">
+        <v>47</v>
+      </c>
+      <c r="AK2" s="134" t="s">
         <v>48</v>
-      </c>
-      <c r="AK2" s="134" t="s">
-        <v>49</v>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="3" spans="1:40">
@@ -1981,45 +1982,45 @@
         <v/>
       </c>
       <c r="Q3" s="136" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V3" s="135" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AA3" s="135" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AF3" s="135" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:40">
       <c r="A4" s="130" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="29">
         <f>IF(Input!C9="Y","Host","Cash")</f>
         <v/>
       </c>
       <c r="E4" s="128" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="97" t="s">
         <v>51</v>
-      </c>
-      <c r="H4" s="97" t="s">
-        <v>52</v>
       </c>
       <c r="I4" s="97" t="n"/>
       <c r="J4" s="98" t="n"/>
       <c r="K4" s="97" t="s">
+        <v>52</v>
+      </c>
+      <c r="L4" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="L4" s="97" t="s">
-        <v>54</v>
-      </c>
       <c r="M4" s="97" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N4" s="128" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q4" s="53" t="n"/>
       <c r="R4" s="53" t="n"/>
@@ -2040,122 +2041,122 @@
     </row>
     <row r="5" spans="1:40">
       <c r="A5" s="130" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="133">
         <f>Input!C8</f>
         <v/>
       </c>
       <c r="E5" s="128" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="128" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="128" t="s">
+      <c r="G5" s="128" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="128" t="s">
+      <c r="H5" s="100" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="100" t="s">
+      <c r="I5" s="100" t="s">
         <v>58</v>
-      </c>
-      <c r="I5" s="100" t="s">
-        <v>59</v>
       </c>
       <c r="J5" s="98" t="n"/>
       <c r="K5" s="100" t="s">
+        <v>59</v>
+      </c>
+      <c r="L5" s="100" t="s">
+        <v>59</v>
+      </c>
+      <c r="M5" s="100" t="s">
         <v>60</v>
       </c>
-      <c r="L5" s="100" t="s">
-        <v>60</v>
-      </c>
-      <c r="M5" s="100" t="s">
+      <c r="N5" s="128" t="s">
         <v>61</v>
       </c>
-      <c r="N5" s="128" t="s">
+      <c r="O5" s="128" t="s">
         <v>62</v>
       </c>
-      <c r="O5" s="128" t="s">
-        <v>63</v>
-      </c>
       <c r="Q5" s="135" t="s">
+        <v>54</v>
+      </c>
+      <c r="R5" s="135" t="s">
         <v>55</v>
       </c>
-      <c r="R5" s="135" t="s">
+      <c r="S5" s="135" t="s">
         <v>56</v>
       </c>
-      <c r="S5" s="135" t="s">
-        <v>57</v>
-      </c>
       <c r="T5" s="135" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V5" s="135" t="s">
+        <v>54</v>
+      </c>
+      <c r="W5" s="135" t="s">
         <v>55</v>
       </c>
-      <c r="W5" s="135" t="s">
+      <c r="X5" s="135" t="s">
         <v>56</v>
       </c>
-      <c r="X5" s="135" t="s">
-        <v>57</v>
-      </c>
       <c r="Y5" s="135" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA5" s="135" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB5" s="135" t="s">
         <v>55</v>
       </c>
-      <c r="AB5" s="135" t="s">
+      <c r="AC5" s="135" t="s">
         <v>56</v>
       </c>
-      <c r="AC5" s="135" t="s">
-        <v>57</v>
-      </c>
       <c r="AD5" s="135" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF5" s="135" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG5" s="135" t="s">
         <v>55</v>
       </c>
-      <c r="AG5" s="135" t="s">
+      <c r="AH5" s="135" t="s">
         <v>56</v>
       </c>
-      <c r="AH5" s="135" t="s">
-        <v>57</v>
-      </c>
       <c r="AI5" s="135" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AK5" s="104" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AL5" s="134" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AM5" s="134" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AN5" s="101" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row customHeight="1" ht="14.1" r="6" spans="1:40">
       <c r="A6" s="129" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="132" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="132" t="s">
+      <c r="C6" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="D6" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="47" t="n">
-        <v>0</v>
+      <c r="F6" s="47" t="s">
+        <v>67</v>
       </c>
       <c r="G6" s="32">
         <f>E6-F6</f>
@@ -2272,10 +2273,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="7" spans="1:40">
       <c r="C7" s="31" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="47" t="n">
         <v>0</v>
@@ -2398,10 +2399,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="8" spans="1:40">
       <c r="C8" s="31" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" s="47" t="n">
         <v>0</v>
@@ -2524,10 +2525,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="9" spans="1:40">
       <c r="C9" s="31" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" s="47" t="n">
         <v>0</v>
@@ -2650,13 +2651,13 @@
     </row>
     <row customHeight="1" ht="14.1" r="10" spans="1:40">
       <c r="B10" s="121" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10" s="47" t="n">
         <v>0</v>
@@ -2779,10 +2780,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="11" spans="1:40">
       <c r="C11" s="31" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" s="47" t="n">
         <v>0</v>
@@ -2905,10 +2906,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="12" spans="1:40">
       <c r="C12" s="31" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E12" s="47" t="n">
         <v>0</v>
@@ -3031,13 +3032,13 @@
     </row>
     <row customHeight="1" ht="14.1" r="13" spans="1:40">
       <c r="B13" s="132" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" s="47" t="n">
         <v>0</v>
@@ -3160,10 +3161,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="14" spans="1:40">
       <c r="C14" s="31" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14" s="47" t="n">
         <v>0</v>
@@ -3286,10 +3287,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="15" spans="1:40">
       <c r="C15" s="31" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E15" s="47" t="n">
         <v>0</v>
@@ -3412,13 +3413,13 @@
     </row>
     <row customHeight="1" ht="14.1" r="16" spans="1:40">
       <c r="B16" s="121" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" s="47" t="n">
         <v>0</v>
@@ -3541,10 +3542,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="17" spans="1:40">
       <c r="C17" s="31" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E17" s="47" t="n">
         <v>0</v>
@@ -3667,10 +3668,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="18" spans="1:40">
       <c r="C18" s="31" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E18" s="47" t="n">
         <v>0</v>
@@ -3793,13 +3794,13 @@
     </row>
     <row customHeight="1" ht="14.1" r="19" spans="1:40">
       <c r="B19" s="121" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E19" s="47" t="n">
         <v>0</v>
@@ -3922,10 +3923,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="20" spans="1:40">
       <c r="C20" s="31" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E20" s="47" t="n">
         <v>0</v>
@@ -4048,13 +4049,13 @@
     </row>
     <row customHeight="1" ht="14.1" r="21" spans="1:40">
       <c r="B21" s="132" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E21" s="47" t="n">
         <v>0</v>
@@ -4177,10 +4178,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="22" spans="1:40">
       <c r="C22" s="31" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E22" s="47" t="n">
         <v>0</v>
@@ -4303,13 +4304,13 @@
     </row>
     <row customHeight="1" ht="14.1" r="23" spans="1:40">
       <c r="B23" s="132" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E23" s="47" t="n">
         <v>0</v>
@@ -4432,10 +4433,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="24" spans="1:40">
       <c r="C24" s="31" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E24" s="47" t="n">
         <v>0</v>
@@ -4558,13 +4559,13 @@
     </row>
     <row customHeight="1" ht="14.1" r="25" spans="1:40">
       <c r="B25" s="121" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E25" s="47" t="n">
         <v>0</v>
@@ -4687,10 +4688,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="26" spans="1:40">
       <c r="C26" s="31" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E26" s="47" t="n">
         <v>0</v>
@@ -4813,10 +4814,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="27" spans="1:40">
       <c r="C27" s="31" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E27" s="47" t="n">
         <v>0</v>
@@ -4939,10 +4940,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="28" spans="1:40">
       <c r="C28" s="31" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D28" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E28" s="47" t="n">
         <v>0</v>
@@ -5065,13 +5066,13 @@
     </row>
     <row customHeight="1" ht="14.1" r="29" spans="1:40">
       <c r="B29" s="123" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C29" s="105" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E29" s="47" t="n">
         <v>0</v>
@@ -5194,10 +5195,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="30" spans="1:40">
       <c r="C30" s="48" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E30" s="47" t="n">
         <v>0</v>
@@ -5320,10 +5321,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="31" spans="1:40">
       <c r="C31" s="105" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E31" s="47" t="n">
         <v>0</v>
@@ -5446,10 +5447,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="32" spans="1:40">
       <c r="C32" s="105" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E32" s="47" t="n">
         <v>0</v>
@@ -5591,10 +5592,10 @@
       <c r="A34" s="35" t="n"/>
       <c r="B34" s="35" t="n"/>
       <c r="C34" s="44" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D34" s="44" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E34" s="32">
         <f>Q34</f>
@@ -5669,7 +5670,7 @@
       <c r="B35" s="35" t="n"/>
       <c r="C35" s="35" t="n"/>
       <c r="D35" s="44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E35" s="32">
         <f>V35</f>
@@ -5728,7 +5729,7 @@
       <c r="B36" s="35" t="n"/>
       <c r="C36" s="35" t="n"/>
       <c r="D36" s="44" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E36" s="32">
         <f>AA36</f>
@@ -5791,7 +5792,7 @@
       <c r="B37" s="35" t="n"/>
       <c r="C37" s="35" t="n"/>
       <c r="D37" s="44" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E37" s="32">
         <f>AF37</f>
@@ -5854,7 +5855,7 @@
       <c r="B38" s="35" t="n"/>
       <c r="C38" s="35" t="n"/>
       <c r="D38" s="44" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E38" s="32">
         <f>SUM(E34:E37)</f>
@@ -5909,27 +5910,27 @@
       <c r="N39" s="35" t="n"/>
       <c r="O39" s="35" t="n"/>
       <c r="Q39" s="134" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V39" s="134" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AK39" s="134" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AL39" s="134" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row customHeight="1" ht="14.1" r="40" spans="1:40">
       <c r="A40" s="129" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B40" s="116" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E40" s="50" t="n">
         <v>0</v>
@@ -6011,10 +6012,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="41" spans="1:40">
       <c r="B41" s="119" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D41" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E41" s="50" t="n">
         <v>0</v>
@@ -6097,10 +6098,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="42" spans="1:40">
       <c r="B42" s="119" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D42" s="31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E42" s="50" t="n">
         <v>0</v>
@@ -6183,10 +6184,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="43" spans="1:40">
       <c r="B43" s="119" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D43" s="31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E43" s="50" t="n">
         <v>0</v>
@@ -6269,10 +6270,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="44" spans="1:40">
       <c r="B44" s="119" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D44" s="31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E44" s="50" t="n">
         <v>0</v>
@@ -6355,10 +6356,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="45" spans="1:40">
       <c r="B45" s="119" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D45" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E45" s="50" t="n">
         <v>0</v>
@@ -6441,10 +6442,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="46" spans="1:40">
       <c r="B46" s="119" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D46" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E46" s="50" t="n">
         <v>0</v>
@@ -6527,10 +6528,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="47" spans="1:40">
       <c r="B47" s="119" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D47" s="31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E47" s="50" t="n">
         <v>0</v>
@@ -6613,10 +6614,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="48" spans="1:40">
       <c r="B48" s="119" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D48" s="31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E48" s="50" t="n">
         <v>0</v>
@@ -6699,10 +6700,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="49" spans="1:40">
       <c r="B49" s="119" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D49" s="31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E49" s="50" t="n">
         <v>0</v>
@@ -6785,10 +6786,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="50" spans="1:40">
       <c r="B50" s="119" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D50" s="31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E50" s="50" t="n">
         <v>0</v>
@@ -6872,7 +6873,7 @@
     <row customHeight="1" ht="14.1" r="51" spans="1:40">
       <c r="B51" s="126" t="n"/>
       <c r="D51" s="31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E51" s="50" t="n"/>
       <c r="F51" s="50" t="n"/>
@@ -6952,7 +6953,7 @@
     <row customHeight="1" ht="14.1" r="52" spans="1:40">
       <c r="B52" s="126" t="n"/>
       <c r="D52" s="31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E52" s="50" t="n"/>
       <c r="F52" s="50" t="n"/>
@@ -7050,10 +7051,10 @@
       <c r="A54" s="35" t="n"/>
       <c r="B54" s="35" t="n"/>
       <c r="C54" s="43" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D54" s="44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E54" s="41">
         <f>Q54</f>
@@ -7120,7 +7121,7 @@
       <c r="B55" s="35" t="n"/>
       <c r="C55" s="35" t="n"/>
       <c r="D55" s="44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E55" s="41">
         <f>V55</f>
@@ -7179,7 +7180,7 @@
       <c r="B56" s="35" t="n"/>
       <c r="C56" s="35" t="n"/>
       <c r="D56" s="44" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E56" s="41">
         <f>SUM(E54:E55)</f>
@@ -7234,18 +7235,18 @@
       <c r="N57" s="35" t="n"/>
       <c r="O57" s="35" t="n"/>
       <c r="AK57" s="134" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row customHeight="1" ht="14.1" r="58" spans="1:40">
       <c r="A58" s="129" t="s">
+        <v>117</v>
+      </c>
+      <c r="B58" s="116" t="s">
+        <v>35</v>
+      </c>
+      <c r="D58" s="44" t="s">
         <v>116</v>
-      </c>
-      <c r="B58" s="116" t="s">
-        <v>36</v>
-      </c>
-      <c r="D58" s="44" t="s">
-        <v>115</v>
       </c>
       <c r="E58" s="47" t="n">
         <v>0</v>
@@ -7308,10 +7309,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="59" spans="1:40">
       <c r="B59" s="116" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D59" s="44" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E59" s="47" t="n">
         <v>0</v>
@@ -7374,10 +7375,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="60" spans="1:40">
       <c r="B60" s="116" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D60" s="44" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E60" s="47" t="n">
         <v>0</v>
@@ -7440,17 +7441,13 @@
     </row>
     <row customHeight="1" ht="14.1" r="61" spans="1:40">
       <c r="B61" s="116" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D61" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="E61" s="106" t="n">
-        <v>0</v>
-      </c>
-      <c r="F61" s="47" t="n">
-        <v>0</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="E61" s="106" t="n"/>
+      <c r="F61" s="47" t="n"/>
       <c r="G61" s="32">
         <f>E61-F61</f>
         <v/>
@@ -7506,10 +7503,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="62" spans="1:40">
       <c r="B62" s="116" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D62" s="44" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E62" s="47" t="n">
         <v>0</v>
@@ -7571,10 +7568,10 @@
     </row>
     <row customHeight="1" ht="14.1" r="63" spans="1:40">
       <c r="B63" s="116" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D63" s="44" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E63" s="47" t="n">
         <v>0</v>
@@ -7656,10 +7653,10 @@
       <c r="A65" s="35" t="n"/>
       <c r="B65" s="35" t="n"/>
       <c r="C65" s="43" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D65" s="44" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E65" s="32">
         <f>Q65</f>
@@ -7722,7 +7719,7 @@
       <c r="B66" s="35" t="n"/>
       <c r="C66" s="35" t="n"/>
       <c r="D66" s="44" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E66" s="32">
         <f>SUM(E65:E65)</f>
@@ -7773,7 +7770,7 @@
     </row>
     <row customHeight="1" ht="14.1" r="68" spans="1:40">
       <c r="A68" s="45" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B68" s="46" t="n"/>
       <c r="C68" s="116">
@@ -7789,28 +7786,28 @@
     </row>
     <row customFormat="1" hidden="1" r="70" s="52" spans="1:40">
       <c r="B70" s="52" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C70" s="52" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row customFormat="1" hidden="1" r="71" s="52" spans="1:40">
       <c r="B71" s="52" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C71" s="52" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row customFormat="1" hidden="1" r="72" s="52" spans="1:40">
       <c r="B72" s="52" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row customFormat="1" hidden="1" r="73" s="52" spans="1:40">
       <c r="B73" s="103" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -7918,7 +7915,7 @@
   <sheetData>
     <row customHeight="1" ht="15.75" r="1" spans="1:15">
       <c r="A1" s="137" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E1" s="65" t="n"/>
       <c r="F1" s="68" t="n"/>
@@ -7947,18 +7944,18 @@
     <row customHeight="1" ht="6.95" r="4" spans="1:15"/>
     <row r="5" spans="1:15">
       <c r="B5" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="21" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B6" s="18">
         <f>ROUND(Point!G34*Point!L34,0)</f>
@@ -7975,7 +7972,7 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="21" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B7" s="18">
         <f>ROUND(Point!G35*Point!L35,0)</f>
@@ -7992,7 +7989,7 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="21" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B8" s="18">
         <f>ROUND(Point!G36*Point!L36,0)</f>
@@ -8009,7 +8006,7 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="21" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B9" s="18">
         <f>ROUND(Point!G37*Point!L37,0)</f>
@@ -8026,7 +8023,7 @@
     </row>
     <row customFormat="1" r="10" s="74" spans="1:15">
       <c r="A10" s="70" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B10" s="71">
         <f>SUM(B6:B9)</f>
@@ -8050,7 +8047,7 @@
     <row customHeight="1" ht="6.95" r="11" spans="1:15"/>
     <row r="12" spans="1:15">
       <c r="A12" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="18">
         <f>ROUND(Point!G54*Point!L54,0)</f>
@@ -8067,7 +8064,7 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" s="18">
         <f>ROUND(Point!G55*Point!L55,0)</f>
@@ -8084,7 +8081,7 @@
     </row>
     <row customFormat="1" r="14" s="74" spans="1:15">
       <c r="A14" s="70" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B14" s="71">
         <f>SUM(B12:B13)</f>
@@ -8108,7 +8105,7 @@
     <row customHeight="1" ht="6.95" r="15" spans="1:15"/>
     <row r="16" spans="1:15">
       <c r="A16" s="21" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B16" s="18">
         <f>ROUND(Point!G58*Point!L58,0)</f>
@@ -8125,7 +8122,7 @@
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="21" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B17" s="18">
         <f>ROUND(Point!G59*Point!L59,0)</f>
@@ -8142,7 +8139,7 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="21" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B18" s="18">
         <f>ROUND(Point!G60*Point!L60,0)</f>
@@ -8159,7 +8156,7 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="21" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B19" s="18">
         <f>ROUND(Point!G61*Point!L61,0)</f>
@@ -8176,7 +8173,7 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" s="21" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B20" s="18">
         <f>ROUND(Point!G62*Point!L62,0)</f>
@@ -8193,7 +8190,7 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="21" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B21" s="18">
         <f>ROUND(Point!G63*Point!L63,0)</f>
@@ -8210,7 +8207,7 @@
     </row>
     <row customFormat="1" r="22" s="74" spans="1:15">
       <c r="A22" s="70" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B22" s="71">
         <f>SUM(B16:B21)</f>
@@ -8234,11 +8231,11 @@
     <row customHeight="1" ht="6.95" r="23" spans="1:15"/>
     <row r="24" spans="1:15">
       <c r="A24" s="75" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24" s="76" t="n"/>
       <c r="C24" s="77" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D24" s="160">
         <f>ROUND(SUM(D10,D14,D22),2)</f>
@@ -8255,7 +8252,7 @@
         <v/>
       </c>
       <c r="C25" s="77" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D25" s="159">
         <f>IF(Input!C9="Y",ROUND(Summary!D24*B25,2),0)</f>
@@ -8264,14 +8261,14 @@
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="75" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B26" s="80">
         <f>Input!C10</f>
         <v/>
       </c>
       <c r="C26" s="77" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D26" s="159">
         <f>ROUND(SUM(D24:D25)*B26,2)</f>
@@ -8285,7 +8282,7 @@
       </c>
       <c r="B27" s="76" t="n"/>
       <c r="C27" s="77" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D27" s="159">
         <f>SUM(D24:D26)</f>
@@ -8294,11 +8291,11 @@
     </row>
     <row r="28" spans="1:15">
       <c r="A28" s="75" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B28" s="76" t="n"/>
       <c r="C28" s="77" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D28" s="159">
         <f>Input!C12</f>
@@ -8312,7 +8309,7 @@
       </c>
       <c r="B29" s="76" t="n"/>
       <c r="C29" s="77" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D29" s="159">
         <f>IF(Input!C9="Y",Summary!D27,0)</f>
@@ -8322,7 +8319,7 @@
     <row r="30" spans="1:15">
       <c r="B30" s="76" t="n"/>
       <c r="C30" s="77" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D30" s="159">
         <f>D29+D28-D27</f>
@@ -8338,25 +8335,25 @@
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="140" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row customHeight="1" ht="6.95" r="34" spans="1:15"/>
     <row r="35" spans="1:15">
       <c r="A35" s="140" t="n"/>
       <c r="B35" s="83" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C35" s="71" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D35" s="71" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:15">
       <c r="A36" s="21" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B36" s="158">
         <f>D6</f>
@@ -8373,7 +8370,7 @@
     </row>
     <row r="37" spans="1:15">
       <c r="A37" s="21" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B37" s="158">
         <f>D7</f>
@@ -8390,7 +8387,7 @@
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="21" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B38" s="158">
         <f>D8</f>
@@ -8407,7 +8404,7 @@
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="21" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B39" s="158">
         <f>D9</f>
@@ -8424,7 +8421,7 @@
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="70" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B40" s="160">
         <f>SUM(B36:B39)</f>
@@ -8442,7 +8439,7 @@
     <row customHeight="1" ht="6.95" r="41" spans="1:15"/>
     <row r="42" spans="1:15">
       <c r="A42" s="70" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B42" s="86">
         <f>Input!D19</f>
@@ -8454,7 +8451,7 @@
     <row customHeight="1" ht="6.95" r="43" spans="1:15"/>
     <row r="44" spans="1:15">
       <c r="A44" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" s="158">
         <f>D12</f>
@@ -8471,7 +8468,7 @@
     </row>
     <row r="45" spans="1:15">
       <c r="A45" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" s="158">
         <f>D13</f>
@@ -8488,7 +8485,7 @@
     </row>
     <row r="46" spans="1:15">
       <c r="A46" s="70" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B46" s="160">
         <f>SUM(B44:B45)</f>
@@ -8506,7 +8503,7 @@
     <row customHeight="1" ht="6.95" r="47" spans="1:15"/>
     <row r="48" spans="1:15">
       <c r="A48" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B48" s="158">
         <f>D22</f>
@@ -8523,7 +8520,7 @@
     </row>
     <row r="49" spans="1:15">
       <c r="A49" s="70" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B49" s="160">
         <f>SUM(B48:B48)</f>
@@ -8541,7 +8538,7 @@
     <row customHeight="1" ht="6.95" r="50" spans="1:15"/>
     <row r="51" spans="1:15">
       <c r="A51" s="89" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B51" s="160">
         <f>B40+B46+B49</f>
@@ -8558,7 +8555,7 @@
     </row>
     <row customFormat="1" hidden="1" r="55" s="68" spans="1:15">
       <c r="F55" s="90" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G55" s="162">
         <f>Input!C12</f>
@@ -8567,7 +8564,7 @@
     </row>
     <row customFormat="1" hidden="1" r="56" s="68" spans="1:15">
       <c r="F56" s="90" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G56" s="162">
         <f>ROUND(IF(Input!C10=0,0,G55-(G55/(1+Input!C10))),2)</f>
@@ -8576,7 +8573,7 @@
     </row>
     <row customFormat="1" hidden="1" r="57" s="68" spans="1:15">
       <c r="F57" s="90" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G57" s="162">
         <f>D14</f>
@@ -8585,7 +8582,7 @@
     </row>
     <row customFormat="1" hidden="1" r="58" s="68" spans="1:15">
       <c r="F58" s="90" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G58" s="162">
         <f>D22</f>
@@ -8594,7 +8591,7 @@
     </row>
     <row customFormat="1" hidden="1" r="59" s="68" spans="1:15">
       <c r="F59" s="90" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G59" s="162">
         <f>G55-SUM(G56:G58)</f>
@@ -8603,7 +8600,7 @@
     </row>
     <row customFormat="1" hidden="1" r="60" s="68" spans="1:15">
       <c r="F60" s="90" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G60" s="162">
         <f>G55-SUM(G56:G59)</f>
@@ -8615,7 +8612,7 @@
     </row>
     <row customFormat="1" hidden="1" r="62" s="68" spans="1:15">
       <c r="F62" s="90" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G62" s="162">
         <f>G59</f>
@@ -8624,7 +8621,7 @@
     </row>
     <row customFormat="1" hidden="1" r="63" s="68" spans="1:15">
       <c r="F63" s="90" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G63" s="93">
         <f>Point!G38</f>
@@ -8633,7 +8630,7 @@
     </row>
     <row customFormat="1" hidden="1" r="64" s="68" spans="1:15">
       <c r="F64" s="90" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G64" s="93">
         <f>26.40825/G62*G63</f>
@@ -8643,24 +8640,24 @@
     <row customFormat="1" hidden="1" r="65" s="68" spans="1:15"/>
     <row customFormat="1" hidden="1" r="66" s="68" spans="1:15">
       <c r="G66" s="94" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H66" s="94" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I66" s="94" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="K66" s="94" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N66" s="94" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row customFormat="1" hidden="1" r="67" s="68" spans="1:15">
       <c r="F67" s="90" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G67" s="93">
         <f>Point!G34</f>
@@ -8697,7 +8694,7 @@
     </row>
     <row customFormat="1" hidden="1" r="68" s="68" spans="1:15">
       <c r="F68" s="90" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G68" s="93">
         <f>Point!G35</f>
@@ -8734,7 +8731,7 @@
     </row>
     <row customFormat="1" hidden="1" r="69" s="68" spans="1:15">
       <c r="F69" s="90" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G69" s="93">
         <f>Point!G36</f>
@@ -8771,7 +8768,7 @@
     </row>
     <row customFormat="1" hidden="1" r="70" s="68" spans="1:15">
       <c r="F70" s="90" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G70" s="93">
         <f>Point!G37</f>
@@ -8886,14 +8883,14 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B1" s="2">
         <f>Input!C5</f>
         <v/>
       </c>
       <c r="D1" s="141" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -8906,7 +8903,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B3" s="2">
         <f>Summary!A25</f>
@@ -8919,7 +8916,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B4" s="2">
         <f>Input!C6</f>
@@ -8934,22 +8931,22 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B6" s="166">
         <f>Summary!D10</f>
         <v/>
       </c>
       <c r="F6" s="167" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G6" s="167" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B7" s="166">
         <f>Summary!D14</f>
@@ -8959,7 +8956,7 @@
         <v>454598</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F7" s="168">
         <f>G13</f>
@@ -8969,7 +8966,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B8" s="166">
         <f>Summary!D22</f>
@@ -8979,7 +8976,7 @@
         <v>464691</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F8" s="168" t="n"/>
       <c r="G8" s="168">
@@ -8994,7 +8991,7 @@
         <v>464692</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F9" s="168" t="n"/>
       <c r="G9" s="168">
@@ -9007,7 +9004,7 @@
         <v>464693</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F10" s="168" t="n"/>
       <c r="G10" s="168">
@@ -9017,7 +9014,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B11" s="166">
         <f>Summary!C40</f>
@@ -9027,7 +9024,7 @@
         <v>454598</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F11" s="168" t="n"/>
       <c r="G11" s="168">
@@ -9037,7 +9034,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B12" s="166">
         <f>+Summary!C46</f>
@@ -9047,7 +9044,7 @@
         <v>202220</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F12" s="168" t="n"/>
       <c r="G12" s="168">
@@ -9057,7 +9054,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B13" s="166">
         <f>+Summary!C49</f>
@@ -9080,20 +9077,20 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B17" s="9">
         <f>Point!G8</f>
         <v/>
       </c>
       <c r="D17" s="62" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E17" s="62" t="n"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B18" s="9">
         <f>Point!G25</f>
@@ -9110,7 +9107,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B19" s="9">
         <f>Point!G10</f>
@@ -9127,7 +9124,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B20" s="9">
         <f>Point!G13</f>
@@ -9144,7 +9141,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B21" s="9">
         <f>Point!G16</f>
@@ -9161,7 +9158,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B22" s="9">
         <f>Point!G6</f>
@@ -9172,7 +9169,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B23" s="9">
         <f>Point!G11</f>
@@ -9189,7 +9186,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B24" s="9">
         <f>Point!G26</f>
@@ -9206,7 +9203,7 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B25" s="9">
         <f>Point!G12</f>
@@ -9215,7 +9212,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B26" s="9">
         <f>Point!G9</f>
@@ -9224,7 +9221,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B27" s="9">
         <f>Point!G24</f>
@@ -9233,7 +9230,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B28" s="9">
         <f>Point!G19</f>
@@ -9242,7 +9239,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B29" s="9">
         <f>Point!G14</f>
@@ -9251,7 +9248,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B30" s="9">
         <f>Point!G20</f>
@@ -9260,7 +9257,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B31" s="9">
         <f>Point!G22</f>
@@ -9269,7 +9266,7 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B32" s="9">
         <f>Point!G21</f>
@@ -9278,7 +9275,7 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B33" s="9">
         <f>Point!G17</f>
@@ -9287,7 +9284,7 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B34" s="9">
         <f>Point!G18</f>
@@ -9296,7 +9293,7 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B35" s="9">
         <f>Point!G27</f>
@@ -9305,7 +9302,7 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B36" s="9">
         <f>Point!G23</f>
@@ -9315,7 +9312,7 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B37" s="9">
         <f>Point!G7</f>
@@ -9324,7 +9321,7 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B38" s="9">
         <f>Point!G15</f>
@@ -9333,7 +9330,7 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B39" s="9">
         <f>Point!G28</f>
@@ -9345,7 +9342,7 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B41" s="169">
         <f>Point!G40</f>
@@ -9354,7 +9351,7 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B42" s="169">
         <f>Point!G41</f>
@@ -9364,7 +9361,7 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B43" s="169">
         <f>Point!G42</f>
@@ -9374,7 +9371,7 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B44" s="169">
         <f>Point!G43</f>
@@ -9384,7 +9381,7 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B45" s="169">
         <f>Point!G44</f>
@@ -9394,7 +9391,7 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B46" s="169">
         <f>Point!G45</f>
@@ -9403,7 +9400,7 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B47" s="169">
         <f>Point!G46</f>
@@ -9412,7 +9409,7 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B48" s="169">
         <f>Point!G47</f>
@@ -9421,7 +9418,7 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B49" s="169">
         <f>Point!G48</f>
@@ -9430,7 +9427,7 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B50" s="169">
         <f>Point!G49</f>
@@ -9439,7 +9436,7 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B51" s="169">
         <f>Point!G50</f>
@@ -9448,7 +9445,7 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B53" s="9">
         <f>Point!G58</f>
@@ -9457,7 +9454,7 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B54" s="9">
         <f>Point!G59</f>
@@ -9466,7 +9463,7 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B55" s="9">
         <f>Point!G60</f>
@@ -9475,7 +9472,7 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B56" s="9">
         <f>Point!G61</f>
@@ -9484,7 +9481,7 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B57" s="9">
         <f>Point!G62</f>
@@ -9493,7 +9490,7 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="10" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B58" s="9">
         <f>Point!G63</f>

</xml_diff>